<commit_message>
updated gantt w server timeframe
</commit_message>
<xml_diff>
--- a/Docs/Gantt.xlsx
+++ b/Docs/Gantt.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{B3D6DE75-DF5B-40CE-9C21-9B5C6FF1B695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E943BAFA-DD29-468F-B0A4-AF069AA61682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="61">
   <si>
     <t>Cree una programación para un proyecto en esta hoja de cálculo.
 Escriba el título de este proyecto en la celda B1. 
@@ -259,6 +259,9 @@
   </si>
   <si>
     <t>API</t>
+  </si>
+  <si>
+    <t>Remi, Vivienne</t>
   </si>
 </sst>
 </file>
@@ -544,7 +547,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="45">
+  <fills count="46">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -796,8 +799,14 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC0C0C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="17">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -997,6 +1006,71 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </top>
+      <bottom style="medium">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </right>
+      <top style="medium">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </top>
+      <bottom style="medium">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </right>
+      <top style="medium">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </top>
+      <bottom style="medium">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom style="medium">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1069,7 +1143,7 @@
     <xf numFmtId="0" fontId="9" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1316,29 +1390,44 @@
     <xf numFmtId="172" fontId="9" fillId="0" borderId="2" xfId="10">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="12" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="12" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="45" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="9" fillId="0" borderId="3" xfId="9">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
       <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="9" fillId="0" borderId="3" xfId="9">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="12" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="12" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="54">
@@ -1603,10 +1692,10 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
     <mruColors>
+      <color rgb="FFC0C0C0"/>
       <color rgb="FF215881"/>
       <color rgb="FF42648A"/>
       <color rgb="FF969696"/>
-      <color rgb="FFC0C0C0"/>
       <color rgb="FF427FC2"/>
       <color rgb="FF44678E"/>
       <color rgb="FF4A6F9C"/>
@@ -1951,7 +2040,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1998,106 +2087,106 @@
       <c r="B3" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="88" t="s">
+      <c r="C3" s="99" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="89"/>
-      <c r="E3" s="93">
+      <c r="D3" s="100"/>
+      <c r="E3" s="98">
         <v>45857</v>
       </c>
-      <c r="F3" s="93"/>
+      <c r="F3" s="98"/>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="88" t="s">
+      <c r="C4" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="89"/>
+      <c r="D4" s="100"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="90">
+      <c r="I4" s="95">
         <f>I5</f>
         <v>45852</v>
       </c>
-      <c r="J4" s="91"/>
-      <c r="K4" s="91"/>
-      <c r="L4" s="91"/>
-      <c r="M4" s="91"/>
-      <c r="N4" s="91"/>
-      <c r="O4" s="92"/>
-      <c r="P4" s="90">
+      <c r="J4" s="96"/>
+      <c r="K4" s="96"/>
+      <c r="L4" s="96"/>
+      <c r="M4" s="96"/>
+      <c r="N4" s="96"/>
+      <c r="O4" s="97"/>
+      <c r="P4" s="95">
         <f>P5</f>
         <v>45859</v>
       </c>
-      <c r="Q4" s="91"/>
-      <c r="R4" s="91"/>
-      <c r="S4" s="91"/>
-      <c r="T4" s="91"/>
-      <c r="U4" s="91"/>
-      <c r="V4" s="92"/>
-      <c r="W4" s="90">
+      <c r="Q4" s="96"/>
+      <c r="R4" s="96"/>
+      <c r="S4" s="96"/>
+      <c r="T4" s="96"/>
+      <c r="U4" s="96"/>
+      <c r="V4" s="97"/>
+      <c r="W4" s="95">
         <f>W5</f>
         <v>45866</v>
       </c>
-      <c r="X4" s="91"/>
-      <c r="Y4" s="91"/>
-      <c r="Z4" s="91"/>
-      <c r="AA4" s="91"/>
-      <c r="AB4" s="91"/>
-      <c r="AC4" s="92"/>
-      <c r="AD4" s="90">
+      <c r="X4" s="96"/>
+      <c r="Y4" s="96"/>
+      <c r="Z4" s="96"/>
+      <c r="AA4" s="96"/>
+      <c r="AB4" s="96"/>
+      <c r="AC4" s="97"/>
+      <c r="AD4" s="95">
         <f>AD5</f>
         <v>45873</v>
       </c>
-      <c r="AE4" s="91"/>
-      <c r="AF4" s="91"/>
-      <c r="AG4" s="91"/>
-      <c r="AH4" s="91"/>
-      <c r="AI4" s="91"/>
-      <c r="AJ4" s="92"/>
-      <c r="AK4" s="90">
+      <c r="AE4" s="96"/>
+      <c r="AF4" s="96"/>
+      <c r="AG4" s="96"/>
+      <c r="AH4" s="96"/>
+      <c r="AI4" s="96"/>
+      <c r="AJ4" s="97"/>
+      <c r="AK4" s="95">
         <f>AK5</f>
         <v>45880</v>
       </c>
-      <c r="AL4" s="91"/>
-      <c r="AM4" s="91"/>
-      <c r="AN4" s="91"/>
-      <c r="AO4" s="91"/>
-      <c r="AP4" s="91"/>
-      <c r="AQ4" s="92"/>
-      <c r="AR4" s="90">
+      <c r="AL4" s="96"/>
+      <c r="AM4" s="96"/>
+      <c r="AN4" s="96"/>
+      <c r="AO4" s="96"/>
+      <c r="AP4" s="96"/>
+      <c r="AQ4" s="97"/>
+      <c r="AR4" s="95">
         <f>AR5</f>
         <v>45887</v>
       </c>
-      <c r="AS4" s="91"/>
-      <c r="AT4" s="91"/>
-      <c r="AU4" s="91"/>
-      <c r="AV4" s="91"/>
-      <c r="AW4" s="91"/>
-      <c r="AX4" s="92"/>
-      <c r="AY4" s="90">
+      <c r="AS4" s="96"/>
+      <c r="AT4" s="96"/>
+      <c r="AU4" s="96"/>
+      <c r="AV4" s="96"/>
+      <c r="AW4" s="96"/>
+      <c r="AX4" s="97"/>
+      <c r="AY4" s="95">
         <f>AY5</f>
         <v>45894</v>
       </c>
-      <c r="AZ4" s="91"/>
-      <c r="BA4" s="91"/>
-      <c r="BB4" s="91"/>
-      <c r="BC4" s="91"/>
-      <c r="BD4" s="91"/>
-      <c r="BE4" s="92"/>
-      <c r="BF4" s="90">
+      <c r="AZ4" s="96"/>
+      <c r="BA4" s="96"/>
+      <c r="BB4" s="96"/>
+      <c r="BC4" s="96"/>
+      <c r="BD4" s="96"/>
+      <c r="BE4" s="97"/>
+      <c r="BF4" s="95">
         <f>BF5</f>
         <v>45901</v>
       </c>
-      <c r="BG4" s="91"/>
-      <c r="BH4" s="91"/>
-      <c r="BI4" s="91"/>
-      <c r="BJ4" s="91"/>
-      <c r="BK4" s="91"/>
-      <c r="BL4" s="92"/>
+      <c r="BG4" s="96"/>
+      <c r="BH4" s="96"/>
+      <c r="BI4" s="96"/>
+      <c r="BJ4" s="96"/>
+      <c r="BK4" s="96"/>
+      <c r="BL4" s="97"/>
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="46" t="s">
@@ -2809,7 +2898,7 @@
       <c r="A10" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="94" t="s">
+      <c r="B10" s="88" t="s">
         <v>54</v>
       </c>
       <c r="C10" s="53" t="s">
@@ -2836,10 +2925,10 @@
       <c r="K10" s="31"/>
       <c r="L10" s="31"/>
       <c r="M10" s="31"/>
-      <c r="N10" s="31"/>
-      <c r="O10" s="31"/>
-      <c r="P10" s="31"/>
-      <c r="Q10" s="31"/>
+      <c r="N10" s="93"/>
+      <c r="O10" s="93"/>
+      <c r="P10" s="93"/>
+      <c r="Q10" s="93"/>
       <c r="R10" s="31"/>
       <c r="S10" s="31"/>
       <c r="T10" s="31"/>
@@ -2890,28 +2979,38 @@
     </row>
     <row r="11" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="45"/>
-      <c r="B11" s="94" t="s">
+      <c r="B11" s="88" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="53"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="77"/>
-      <c r="F11" s="77"/>
+      <c r="C11" s="53" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="17">
+        <v>0</v>
+      </c>
+      <c r="E11" s="77">
+        <f>Inicio_del_proyecto</f>
+        <v>45857</v>
+      </c>
+      <c r="F11" s="77">
+        <f>E11+7</f>
+        <v>45864</v>
+      </c>
       <c r="G11" s="14"/>
-      <c r="H11" s="14" t="str">
+      <c r="H11" s="14">
         <f t="shared" si="6"/>
-        <v/>
+        <v>8</v>
       </c>
       <c r="I11" s="31"/>
       <c r="J11" s="31"/>
       <c r="K11" s="31"/>
       <c r="L11" s="31"/>
-      <c r="M11" s="31"/>
-      <c r="N11" s="31"/>
-      <c r="O11" s="31"/>
-      <c r="P11" s="31"/>
-      <c r="Q11" s="31"/>
-      <c r="R11" s="31"/>
+      <c r="M11" s="90"/>
+      <c r="N11" s="94"/>
+      <c r="O11" s="94"/>
+      <c r="P11" s="94"/>
+      <c r="Q11" s="94"/>
+      <c r="R11" s="91"/>
       <c r="S11" s="31"/>
       <c r="T11" s="31"/>
       <c r="U11" s="31"/>
@@ -2988,10 +3087,10 @@
       <c r="K12" s="31"/>
       <c r="L12" s="31"/>
       <c r="M12" s="31"/>
-      <c r="N12" s="31"/>
-      <c r="O12" s="31"/>
-      <c r="P12" s="31"/>
-      <c r="Q12" s="31"/>
+      <c r="N12" s="92"/>
+      <c r="O12" s="92"/>
+      <c r="P12" s="92"/>
+      <c r="Q12" s="92"/>
       <c r="R12" s="31"/>
       <c r="S12" s="31"/>
       <c r="T12" s="31"/>
@@ -4198,7 +4297,7 @@
     </row>
     <row r="29" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="45"/>
-      <c r="B29" s="95" t="s">
+      <c r="B29" s="89" t="s">
         <v>58</v>
       </c>
       <c r="C29" s="59"/>
@@ -4561,17 +4660,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
+    <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="I4:O4"/>
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
-    <mergeCell ref="AY4:BE4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D33">
     <cfRule type="dataBar" priority="14">
@@ -4611,6 +4710,9 @@
   <headerFooter differentFirst="1" scaleWithDoc="0">
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
+  <ignoredErrors>
+    <ignoredError sqref="F10" formula="1"/>
+  </ignoredErrors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
@@ -4739,6 +4841,35 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="24" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2d714a3296df14eba7a100bb665443ca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="49549bf45bfbbfb6cffed527380e77e1" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -5026,36 +5157,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC3AD2E1-977A-4D4F-8EE8-D64B5FFADF75}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4A34E49-7289-4AEA-9593-4F55E04ADB10}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F80F839-78EF-4FF4-A673-3CC84279C232}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5074,24 +5196,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4A34E49-7289-4AEA-9593-4F55E04ADB10}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC3AD2E1-977A-4D4F-8EE8-D64B5FFADF75}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
chore(docs)!: task projection in the Gantt until september 3rd
</commit_message>
<xml_diff>
--- a/Docs/Gantt.xlsx
+++ b/Docs/Gantt.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E943BAFA-DD29-468F-B0A4-AF069AA61682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EBF450A-1CEE-46F2-80D2-D5FAFDDE8215}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="81">
   <si>
     <t>Cree una programación para un proyecto en esta hoja de cálculo.
 Escriba el título de este proyecto en la celda B1. 
@@ -222,9 +222,6 @@
     <t>En este diagrama no se muestran avances previos a la fecha de creación.</t>
   </si>
   <si>
-    <t>Servidor</t>
-  </si>
-  <si>
     <t>AGEBs y SCINCE</t>
   </si>
   <si>
@@ -252,16 +249,79 @@
     <t>Ruy, Arroyo, Remi</t>
   </si>
   <si>
-    <t>Login</t>
-  </si>
-  <si>
-    <t>Interfaz de creación de dashboards</t>
-  </si>
-  <si>
-    <t>API</t>
-  </si>
-  <si>
     <t>Remi, Vivienne</t>
+  </si>
+  <si>
+    <t>Manual de Usuario</t>
+  </si>
+  <si>
+    <t>API RESTful para comunicación local</t>
+  </si>
+  <si>
+    <t>Centralización de datos en servidor</t>
+  </si>
+  <si>
+    <t>Hospedaje del sitio web</t>
+  </si>
+  <si>
+    <t>Servidor setup</t>
+  </si>
+  <si>
+    <t>Framework para integración Python</t>
+  </si>
+  <si>
+    <t>Nuevas fuentes de datos censales</t>
+  </si>
+  <si>
+    <t>Diseño del modelo de datos orientado a grafos</t>
+  </si>
+  <si>
+    <t>Segmentación territorial por ML</t>
+  </si>
+  <si>
+    <t>Clasificación por impacto económico</t>
+  </si>
+  <si>
+    <t>Modelado predictivo de población</t>
+  </si>
+  <si>
+    <t>Análisis de grafos geoespaciales</t>
+  </si>
+  <si>
+    <t>Sistema de login y autenticación</t>
+  </si>
+  <si>
+    <t>Registro y recuperación de contraseña</t>
+  </si>
+  <si>
+    <t>Clusterización por nivel geográfico</t>
+  </si>
+  <si>
+    <t>Filtros interactivos por zona</t>
+  </si>
+  <si>
+    <t>Sistema de dashboards</t>
+  </si>
+  <si>
+    <t>Ítems con visualización de datos</t>
+  </si>
+  <si>
+    <t>Data binding de ítems con filtros</t>
+  </si>
+  <si>
+    <t>Personalización y estilos</t>
+  </si>
+  <si>
+    <t>Comparación entre zonas</t>
+  </si>
+  <si>
+    <t>Visualización de series temporales</t>
+  </si>
+  <si>
+    <t>Exportación de mapas</t>
+  </si>
+  <si>
+    <t>LLM asistente de IA</t>
   </si>
 </sst>
 </file>
@@ -2036,11 +2096,11 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BL36"/>
+  <dimension ref="A1:BL59"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2073,7 +2133,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:64" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="45" t="s">
         <v>1</v>
       </c>
@@ -2751,7 +2811,7 @@
       <c r="F8" s="76"/>
       <c r="G8" s="14"/>
       <c r="H8" s="14" t="str">
-        <f t="shared" ref="H8:H33" si="6">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="H8:H56" si="6">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="I8" s="31"/>
@@ -2899,10 +2959,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="88" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C10" s="53" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D10" s="17">
         <v>0</v>
@@ -2980,10 +3040,10 @@
     <row r="11" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="45"/>
       <c r="B11" s="88" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="C11" s="53" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D11" s="17">
         <v>0</v>
@@ -3061,10 +3121,10 @@
     <row r="12" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="45"/>
       <c r="B12" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="53" t="s">
         <v>55</v>
-      </c>
-      <c r="C12" s="53" t="s">
-        <v>56</v>
       </c>
       <c r="D12" s="17">
         <v>0</v>
@@ -3142,16 +3202,22 @@
     <row r="13" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="45"/>
       <c r="B13" s="61" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C13" s="53"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="77"/>
-      <c r="F13" s="77"/>
+      <c r="D13" s="17">
+        <v>0</v>
+      </c>
+      <c r="E13" s="77">
+        <v>45865</v>
+      </c>
+      <c r="F13" s="77">
+        <v>45869</v>
+      </c>
       <c r="G13" s="14"/>
-      <c r="H13" s="14" t="str">
+      <c r="H13" s="14">
         <f t="shared" si="6"/>
-        <v/>
+        <v>5</v>
       </c>
       <c r="I13" s="31"/>
       <c r="J13" s="31"/>
@@ -3211,21 +3277,22 @@
       <c r="BL13" s="31"/>
     </row>
     <row r="14" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="46" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" s="54"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="78"/>
-      <c r="F14" s="79"/>
+      <c r="A14" s="45"/>
+      <c r="B14" s="61" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="53"/>
+      <c r="D14" s="17">
+        <v>0</v>
+      </c>
+      <c r="E14" s="77">
+        <v>45865</v>
+      </c>
+      <c r="F14" s="77">
+        <v>45867</v>
+      </c>
       <c r="G14" s="14"/>
-      <c r="H14" s="14" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
+      <c r="H14" s="14"/>
       <c r="I14" s="31"/>
       <c r="J14" s="31"/>
       <c r="K14" s="31"/>
@@ -3284,29 +3351,22 @@
       <c r="BL14" s="31"/>
     </row>
     <row r="15" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="46"/>
-      <c r="B15" s="62" t="s">
-        <v>48</v>
-      </c>
-      <c r="C15" s="55" t="s">
-        <v>49</v>
-      </c>
-      <c r="D15" s="20">
-        <v>0.5</v>
-      </c>
-      <c r="E15" s="80">
-        <f>Inicio_del_proyecto</f>
-        <v>45857</v>
-      </c>
-      <c r="F15" s="80">
-        <f>E15+7</f>
-        <v>45864</v>
+      <c r="A15" s="45"/>
+      <c r="B15" s="61" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="53"/>
+      <c r="D15" s="17">
+        <v>0</v>
+      </c>
+      <c r="E15" s="77">
+        <v>45868</v>
+      </c>
+      <c r="F15" s="77">
+        <v>45870</v>
       </c>
       <c r="G15" s="14"/>
-      <c r="H15" s="14">
-        <f t="shared" si="6"/>
-        <v>8</v>
-      </c>
+      <c r="H15" s="14"/>
       <c r="I15" s="31"/>
       <c r="J15" s="31"/>
       <c r="K15" s="31"/>
@@ -3366,16 +3426,13 @@
     </row>
     <row r="16" spans="1:64" s="3" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="45"/>
-      <c r="B16" s="62"/>
-      <c r="C16" s="55"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="80"/>
-      <c r="F16" s="80"/>
+      <c r="B16" s="61"/>
+      <c r="C16" s="53"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="77"/>
+      <c r="F16" s="77"/>
       <c r="G16" s="14"/>
-      <c r="H16" s="14" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
+      <c r="H16" s="14"/>
       <c r="I16" s="31"/>
       <c r="J16" s="31"/>
       <c r="K16" s="31"/>
@@ -3388,8 +3445,8 @@
       <c r="R16" s="31"/>
       <c r="S16" s="31"/>
       <c r="T16" s="31"/>
-      <c r="U16" s="32"/>
-      <c r="V16" s="32"/>
+      <c r="U16" s="31"/>
+      <c r="V16" s="31"/>
       <c r="W16" s="31"/>
       <c r="X16" s="31"/>
       <c r="Y16" s="31"/>
@@ -3435,16 +3492,13 @@
     </row>
     <row r="17" spans="1:64" s="3" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="45"/>
-      <c r="B17" s="62"/>
-      <c r="C17" s="55"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="80"/>
-      <c r="F17" s="80"/>
+      <c r="B17" s="61"/>
+      <c r="C17" s="53"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="77"/>
+      <c r="F17" s="77"/>
       <c r="G17" s="14"/>
-      <c r="H17" s="14" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
+      <c r="H17" s="14"/>
       <c r="I17" s="31"/>
       <c r="J17" s="31"/>
       <c r="K17" s="31"/>
@@ -3504,16 +3558,13 @@
     </row>
     <row r="18" spans="1:64" s="3" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="45"/>
-      <c r="B18" s="62"/>
-      <c r="C18" s="55"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="80"/>
-      <c r="F18" s="80"/>
+      <c r="B18" s="61"/>
+      <c r="C18" s="53"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="77"/>
+      <c r="F18" s="77"/>
       <c r="G18" s="14"/>
-      <c r="H18" s="14" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
+      <c r="H18" s="14"/>
       <c r="I18" s="31"/>
       <c r="J18" s="31"/>
       <c r="K18" s="31"/>
@@ -3530,7 +3581,7 @@
       <c r="V18" s="31"/>
       <c r="W18" s="31"/>
       <c r="X18" s="31"/>
-      <c r="Y18" s="32"/>
+      <c r="Y18" s="31"/>
       <c r="Z18" s="31"/>
       <c r="AA18" s="31"/>
       <c r="AB18" s="31"/>
@@ -3573,16 +3624,13 @@
     </row>
     <row r="19" spans="1:64" s="3" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="45"/>
-      <c r="B19" s="62"/>
-      <c r="C19" s="55"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="80"/>
-      <c r="F19" s="80"/>
+      <c r="B19" s="61"/>
+      <c r="C19" s="53"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="77"/>
+      <c r="F19" s="77"/>
       <c r="G19" s="14"/>
-      <c r="H19" s="14" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
+      <c r="H19" s="14"/>
       <c r="I19" s="31"/>
       <c r="J19" s="31"/>
       <c r="K19" s="31"/>
@@ -3640,22 +3688,15 @@
       <c r="BK19" s="31"/>
       <c r="BL19" s="31"/>
     </row>
-    <row r="20" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="45" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20" s="56"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="81"/>
-      <c r="F20" s="82"/>
+    <row r="20" spans="1:64" s="3" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="45"/>
+      <c r="B20" s="61"/>
+      <c r="C20" s="53"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="77"/>
+      <c r="F20" s="77"/>
       <c r="G20" s="14"/>
-      <c r="H20" s="14" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
+      <c r="H20" s="14"/>
       <c r="I20" s="31"/>
       <c r="J20" s="31"/>
       <c r="K20" s="31"/>
@@ -3714,28 +3755,20 @@
       <c r="BL20" s="31"/>
     </row>
     <row r="21" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="45"/>
-      <c r="B21" s="63" t="s">
-        <v>50</v>
-      </c>
-      <c r="C21" s="57" t="s">
-        <v>51</v>
-      </c>
-      <c r="D21" s="23">
-        <v>0</v>
-      </c>
-      <c r="E21" s="83">
-        <f>Inicio_del_proyecto</f>
-        <v>45857</v>
-      </c>
-      <c r="F21" s="83">
-        <f>E21+7</f>
-        <v>45864</v>
-      </c>
+      <c r="A21" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="54"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="78"/>
+      <c r="F21" s="79"/>
       <c r="G21" s="14"/>
-      <c r="H21" s="14">
+      <c r="H21" s="14" t="str">
         <f t="shared" si="6"/>
-        <v>8</v>
+        <v/>
       </c>
       <c r="I21" s="31"/>
       <c r="J21" s="31"/>
@@ -3794,17 +3827,29 @@
       <c r="BK21" s="31"/>
       <c r="BL21" s="31"/>
     </row>
-    <row r="22" spans="1:64" s="3" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="45"/>
-      <c r="B22" s="63"/>
-      <c r="C22" s="57"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="83"/>
-      <c r="F22" s="83"/>
+    <row r="22" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="46"/>
+      <c r="B22" s="62" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="55" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="E22" s="80">
+        <f>Inicio_del_proyecto</f>
+        <v>45857</v>
+      </c>
+      <c r="F22" s="80">
+        <f>E22+7</f>
+        <v>45864</v>
+      </c>
       <c r="G22" s="14"/>
-      <c r="H22" s="14" t="str">
+      <c r="H22" s="14">
         <f t="shared" si="6"/>
-        <v/>
+        <v>8</v>
       </c>
       <c r="I22" s="31"/>
       <c r="J22" s="31"/>
@@ -3863,17 +3908,25 @@
       <c r="BK22" s="31"/>
       <c r="BL22" s="31"/>
     </row>
-    <row r="23" spans="1:64" s="3" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="45"/>
-      <c r="B23" s="63"/>
-      <c r="C23" s="57"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="83"/>
-      <c r="F23" s="83"/>
+      <c r="B23" s="62" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" s="55"/>
+      <c r="D23" s="20">
+        <v>0</v>
+      </c>
+      <c r="E23" s="80">
+        <v>45865</v>
+      </c>
+      <c r="F23" s="80">
+        <v>45869</v>
+      </c>
       <c r="G23" s="14"/>
-      <c r="H23" s="14" t="str">
+      <c r="H23" s="14">
         <f t="shared" si="6"/>
-        <v/>
+        <v>5</v>
       </c>
       <c r="I23" s="31"/>
       <c r="J23" s="31"/>
@@ -3887,8 +3940,8 @@
       <c r="R23" s="31"/>
       <c r="S23" s="31"/>
       <c r="T23" s="31"/>
-      <c r="U23" s="31"/>
-      <c r="V23" s="31"/>
+      <c r="U23" s="32"/>
+      <c r="V23" s="32"/>
       <c r="W23" s="31"/>
       <c r="X23" s="31"/>
       <c r="Y23" s="31"/>
@@ -3932,17 +3985,25 @@
       <c r="BK23" s="31"/>
       <c r="BL23" s="31"/>
     </row>
-    <row r="24" spans="1:64" s="3" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="45"/>
-      <c r="B24" s="63"/>
-      <c r="C24" s="57"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="83"/>
-      <c r="F24" s="83"/>
+      <c r="B24" s="62" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="55"/>
+      <c r="D24" s="20">
+        <v>0</v>
+      </c>
+      <c r="E24" s="80">
+        <v>45870</v>
+      </c>
+      <c r="F24" s="80">
+        <v>45872</v>
+      </c>
       <c r="G24" s="14"/>
-      <c r="H24" s="14" t="str">
+      <c r="H24" s="14">
         <f t="shared" si="6"/>
-        <v/>
+        <v>3</v>
       </c>
       <c r="I24" s="31"/>
       <c r="J24" s="31"/>
@@ -4003,11 +4064,11 @@
     </row>
     <row r="25" spans="1:64" s="3" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="45"/>
-      <c r="B25" s="63"/>
-      <c r="C25" s="57"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="83"/>
-      <c r="F25" s="83"/>
+      <c r="B25" s="62"/>
+      <c r="C25" s="55"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="80"/>
+      <c r="F25" s="80"/>
       <c r="G25" s="14"/>
       <c r="H25" s="14" t="str">
         <f t="shared" si="6"/>
@@ -4029,7 +4090,7 @@
       <c r="V25" s="31"/>
       <c r="W25" s="31"/>
       <c r="X25" s="31"/>
-      <c r="Y25" s="31"/>
+      <c r="Y25" s="32"/>
       <c r="Z25" s="31"/>
       <c r="AA25" s="31"/>
       <c r="AB25" s="31"/>
@@ -4070,17 +4131,13 @@
       <c r="BK25" s="31"/>
       <c r="BL25" s="31"/>
     </row>
-    <row r="26" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="45" t="s">
-        <v>11</v>
-      </c>
-      <c r="B26" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="C26" s="58"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="84"/>
-      <c r="F26" s="85"/>
+    <row r="26" spans="1:64" s="3" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="45"/>
+      <c r="B26" s="62"/>
+      <c r="C26" s="55"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="80"/>
+      <c r="F26" s="80"/>
       <c r="G26" s="14"/>
       <c r="H26" s="14" t="str">
         <f t="shared" si="6"/>
@@ -4144,28 +4201,20 @@
       <c r="BL26" s="31"/>
     </row>
     <row r="27" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="45"/>
-      <c r="B27" s="64" t="s">
-        <v>53</v>
-      </c>
-      <c r="C27" s="59" t="s">
-        <v>52</v>
-      </c>
-      <c r="D27" s="26">
-        <v>0</v>
-      </c>
-      <c r="E27" s="86">
-        <f>Inicio_del_proyecto</f>
-        <v>45857</v>
-      </c>
-      <c r="F27" s="86">
-        <f>E27+7</f>
-        <v>45864</v>
-      </c>
+      <c r="A27" s="45" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C27" s="56"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="81"/>
+      <c r="F27" s="82"/>
       <c r="G27" s="14"/>
-      <c r="H27" s="14">
+      <c r="H27" s="14" t="str">
         <f t="shared" si="6"/>
-        <v>8</v>
+        <v/>
       </c>
       <c r="I27" s="31"/>
       <c r="J27" s="31"/>
@@ -4226,17 +4275,27 @@
     </row>
     <row r="28" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="45"/>
-      <c r="B28" s="64" t="s">
-        <v>57</v>
-      </c>
-      <c r="C28" s="59"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="86"/>
-      <c r="F28" s="86"/>
+      <c r="B28" s="63" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="57" t="s">
+        <v>50</v>
+      </c>
+      <c r="D28" s="23">
+        <v>0</v>
+      </c>
+      <c r="E28" s="83">
+        <f>Inicio_del_proyecto</f>
+        <v>45857</v>
+      </c>
+      <c r="F28" s="83">
+        <f>E28+7</f>
+        <v>45864</v>
+      </c>
       <c r="G28" s="14"/>
-      <c r="H28" s="14" t="str">
+      <c r="H28" s="14">
         <f t="shared" si="6"/>
-        <v/>
+        <v>8</v>
       </c>
       <c r="I28" s="31"/>
       <c r="J28" s="31"/>
@@ -4297,18 +4356,23 @@
     </row>
     <row r="29" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="45"/>
-      <c r="B29" s="89" t="s">
-        <v>58</v>
-      </c>
-      <c r="C29" s="59"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="86"/>
-      <c r="F29" s="86"/>
+      <c r="B29" s="63" t="s">
+        <v>64</v>
+      </c>
+      <c r="C29" s="57"/>
+      <c r="D29" s="23">
+        <v>0</v>
+      </c>
+      <c r="E29" s="83">
+        <f>Inicio_del_proyecto+2</f>
+        <v>45859</v>
+      </c>
+      <c r="F29" s="83">
+        <f>E29+7</f>
+        <v>45866</v>
+      </c>
       <c r="G29" s="14"/>
-      <c r="H29" s="14" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
+      <c r="H29" s="14"/>
       <c r="I29" s="31"/>
       <c r="J29" s="31"/>
       <c r="K29" s="31"/>
@@ -4366,18 +4430,23 @@
       <c r="BK29" s="31"/>
       <c r="BL29" s="31"/>
     </row>
-    <row r="30" spans="1:64" s="3" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="45"/>
-      <c r="B30" s="64"/>
-      <c r="C30" s="59"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="86"/>
-      <c r="F30" s="86"/>
+      <c r="B30" s="63" t="s">
+        <v>65</v>
+      </c>
+      <c r="C30" s="57"/>
+      <c r="D30" s="23">
+        <v>0</v>
+      </c>
+      <c r="E30" s="83">
+        <v>45877</v>
+      </c>
+      <c r="F30" s="83">
+        <v>45881</v>
+      </c>
       <c r="G30" s="14"/>
-      <c r="H30" s="14" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
+      <c r="H30" s="14"/>
       <c r="I30" s="31"/>
       <c r="J30" s="31"/>
       <c r="K30" s="31"/>
@@ -4435,18 +4504,23 @@
       <c r="BK30" s="31"/>
       <c r="BL30" s="31"/>
     </row>
-    <row r="31" spans="1:64" s="3" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="45"/>
-      <c r="B31" s="64"/>
-      <c r="C31" s="59"/>
-      <c r="D31" s="26"/>
-      <c r="E31" s="86"/>
-      <c r="F31" s="86"/>
+      <c r="B31" s="63" t="s">
+        <v>66</v>
+      </c>
+      <c r="C31" s="57"/>
+      <c r="D31" s="23">
+        <v>0</v>
+      </c>
+      <c r="E31" s="83">
+        <v>45882</v>
+      </c>
+      <c r="F31" s="83">
+        <v>45885</v>
+      </c>
       <c r="G31" s="14"/>
-      <c r="H31" s="14" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
+      <c r="H31" s="14"/>
       <c r="I31" s="31"/>
       <c r="J31" s="31"/>
       <c r="K31" s="31"/>
@@ -4505,19 +4579,22 @@
       <c r="BL31" s="31"/>
     </row>
     <row r="32" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="45" t="s">
-        <v>12</v>
-      </c>
-      <c r="B32" s="65"/>
-      <c r="C32" s="60"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="87"/>
-      <c r="F32" s="87"/>
+      <c r="A32" s="45"/>
+      <c r="B32" s="63" t="s">
+        <v>67</v>
+      </c>
+      <c r="C32" s="57"/>
+      <c r="D32" s="23">
+        <v>0</v>
+      </c>
+      <c r="E32" s="83">
+        <v>45886</v>
+      </c>
+      <c r="F32" s="83">
+        <v>45891</v>
+      </c>
       <c r="G32" s="14"/>
-      <c r="H32" s="14" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
+      <c r="H32" s="14"/>
       <c r="I32" s="31"/>
       <c r="J32" s="31"/>
       <c r="K32" s="31"/>
@@ -4576,87 +4653,1759 @@
       <c r="BL32" s="31"/>
     </row>
     <row r="33" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="46" t="s">
-        <v>13</v>
-      </c>
-      <c r="B33" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="C33" s="28"/>
-      <c r="D33" s="29"/>
-      <c r="E33" s="70"/>
-      <c r="F33" s="71"/>
-      <c r="G33" s="30"/>
-      <c r="H33" s="30" t="str">
+      <c r="A33" s="45"/>
+      <c r="B33" s="63" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" s="57"/>
+      <c r="D33" s="23">
+        <v>0</v>
+      </c>
+      <c r="E33" s="83">
+        <v>45892</v>
+      </c>
+      <c r="F33" s="83">
+        <v>45896</v>
+      </c>
+      <c r="G33" s="14"/>
+      <c r="H33" s="14"/>
+      <c r="I33" s="31"/>
+      <c r="J33" s="31"/>
+      <c r="K33" s="31"/>
+      <c r="L33" s="31"/>
+      <c r="M33" s="31"/>
+      <c r="N33" s="31"/>
+      <c r="O33" s="31"/>
+      <c r="P33" s="31"/>
+      <c r="Q33" s="31"/>
+      <c r="R33" s="31"/>
+      <c r="S33" s="31"/>
+      <c r="T33" s="31"/>
+      <c r="U33" s="31"/>
+      <c r="V33" s="31"/>
+      <c r="W33" s="31"/>
+      <c r="X33" s="31"/>
+      <c r="Y33" s="31"/>
+      <c r="Z33" s="31"/>
+      <c r="AA33" s="31"/>
+      <c r="AB33" s="31"/>
+      <c r="AC33" s="31"/>
+      <c r="AD33" s="31"/>
+      <c r="AE33" s="31"/>
+      <c r="AF33" s="31"/>
+      <c r="AG33" s="31"/>
+      <c r="AH33" s="31"/>
+      <c r="AI33" s="31"/>
+      <c r="AJ33" s="31"/>
+      <c r="AK33" s="31"/>
+      <c r="AL33" s="31"/>
+      <c r="AM33" s="31"/>
+      <c r="AN33" s="31"/>
+      <c r="AO33" s="31"/>
+      <c r="AP33" s="31"/>
+      <c r="AQ33" s="31"/>
+      <c r="AR33" s="31"/>
+      <c r="AS33" s="31"/>
+      <c r="AT33" s="31"/>
+      <c r="AU33" s="31"/>
+      <c r="AV33" s="31"/>
+      <c r="AW33" s="31"/>
+      <c r="AX33" s="31"/>
+      <c r="AY33" s="31"/>
+      <c r="AZ33" s="31"/>
+      <c r="BA33" s="31"/>
+      <c r="BB33" s="31"/>
+      <c r="BC33" s="31"/>
+      <c r="BD33" s="31"/>
+      <c r="BE33" s="31"/>
+      <c r="BF33" s="31"/>
+      <c r="BG33" s="31"/>
+      <c r="BH33" s="31"/>
+      <c r="BI33" s="31"/>
+      <c r="BJ33" s="31"/>
+      <c r="BK33" s="31"/>
+      <c r="BL33" s="31"/>
+    </row>
+    <row r="34" spans="1:64" s="3" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="45"/>
+      <c r="B34" s="63"/>
+      <c r="C34" s="57"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="83"/>
+      <c r="F34" s="83"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="14" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="I33" s="33"/>
-      <c r="J33" s="33"/>
-      <c r="K33" s="33"/>
-      <c r="L33" s="33"/>
-      <c r="M33" s="33"/>
-      <c r="N33" s="33"/>
-      <c r="O33" s="33"/>
-      <c r="P33" s="33"/>
-      <c r="Q33" s="33"/>
-      <c r="R33" s="33"/>
-      <c r="S33" s="33"/>
-      <c r="T33" s="33"/>
-      <c r="U33" s="33"/>
-      <c r="V33" s="33"/>
-      <c r="W33" s="33"/>
-      <c r="X33" s="33"/>
-      <c r="Y33" s="33"/>
-      <c r="Z33" s="33"/>
-      <c r="AA33" s="33"/>
-      <c r="AB33" s="33"/>
-      <c r="AC33" s="33"/>
-      <c r="AD33" s="33"/>
-      <c r="AE33" s="33"/>
-      <c r="AF33" s="33"/>
-      <c r="AG33" s="33"/>
-      <c r="AH33" s="33"/>
-      <c r="AI33" s="33"/>
-      <c r="AJ33" s="33"/>
-      <c r="AK33" s="33"/>
-      <c r="AL33" s="33"/>
-      <c r="AM33" s="33"/>
-      <c r="AN33" s="33"/>
-      <c r="AO33" s="33"/>
-      <c r="AP33" s="33"/>
-      <c r="AQ33" s="33"/>
-      <c r="AR33" s="33"/>
-      <c r="AS33" s="33"/>
-      <c r="AT33" s="33"/>
-      <c r="AU33" s="33"/>
-      <c r="AV33" s="33"/>
-      <c r="AW33" s="33"/>
-      <c r="AX33" s="33"/>
-      <c r="AY33" s="33"/>
-      <c r="AZ33" s="33"/>
-      <c r="BA33" s="33"/>
-      <c r="BB33" s="33"/>
-      <c r="BC33" s="33"/>
-      <c r="BD33" s="33"/>
-      <c r="BE33" s="33"/>
-      <c r="BF33" s="33"/>
-      <c r="BG33" s="33"/>
-      <c r="BH33" s="33"/>
-      <c r="BI33" s="33"/>
-      <c r="BJ33" s="33"/>
-      <c r="BK33" s="33"/>
-      <c r="BL33" s="33"/>
-    </row>
-    <row r="34" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G34" s="6"/>
-    </row>
-    <row r="35" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C35" s="11"/>
-      <c r="F35" s="47"/>
-    </row>
-    <row r="36" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C36" s="12"/>
+      <c r="I34" s="31"/>
+      <c r="J34" s="31"/>
+      <c r="K34" s="31"/>
+      <c r="L34" s="31"/>
+      <c r="M34" s="31"/>
+      <c r="N34" s="31"/>
+      <c r="O34" s="31"/>
+      <c r="P34" s="31"/>
+      <c r="Q34" s="31"/>
+      <c r="R34" s="31"/>
+      <c r="S34" s="31"/>
+      <c r="T34" s="31"/>
+      <c r="U34" s="31"/>
+      <c r="V34" s="31"/>
+      <c r="W34" s="31"/>
+      <c r="X34" s="31"/>
+      <c r="Y34" s="31"/>
+      <c r="Z34" s="31"/>
+      <c r="AA34" s="31"/>
+      <c r="AB34" s="31"/>
+      <c r="AC34" s="31"/>
+      <c r="AD34" s="31"/>
+      <c r="AE34" s="31"/>
+      <c r="AF34" s="31"/>
+      <c r="AG34" s="31"/>
+      <c r="AH34" s="31"/>
+      <c r="AI34" s="31"/>
+      <c r="AJ34" s="31"/>
+      <c r="AK34" s="31"/>
+      <c r="AL34" s="31"/>
+      <c r="AM34" s="31"/>
+      <c r="AN34" s="31"/>
+      <c r="AO34" s="31"/>
+      <c r="AP34" s="31"/>
+      <c r="AQ34" s="31"/>
+      <c r="AR34" s="31"/>
+      <c r="AS34" s="31"/>
+      <c r="AT34" s="31"/>
+      <c r="AU34" s="31"/>
+      <c r="AV34" s="31"/>
+      <c r="AW34" s="31"/>
+      <c r="AX34" s="31"/>
+      <c r="AY34" s="31"/>
+      <c r="AZ34" s="31"/>
+      <c r="BA34" s="31"/>
+      <c r="BB34" s="31"/>
+      <c r="BC34" s="31"/>
+      <c r="BD34" s="31"/>
+      <c r="BE34" s="31"/>
+      <c r="BF34" s="31"/>
+      <c r="BG34" s="31"/>
+      <c r="BH34" s="31"/>
+      <c r="BI34" s="31"/>
+      <c r="BJ34" s="31"/>
+      <c r="BK34" s="31"/>
+      <c r="BL34" s="31"/>
+    </row>
+    <row r="35" spans="1:64" s="3" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="45"/>
+      <c r="B35" s="63"/>
+      <c r="C35" s="57"/>
+      <c r="D35" s="23"/>
+      <c r="E35" s="83"/>
+      <c r="F35" s="83"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="14" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="I35" s="31"/>
+      <c r="J35" s="31"/>
+      <c r="K35" s="31"/>
+      <c r="L35" s="31"/>
+      <c r="M35" s="31"/>
+      <c r="N35" s="31"/>
+      <c r="O35" s="31"/>
+      <c r="P35" s="31"/>
+      <c r="Q35" s="31"/>
+      <c r="R35" s="31"/>
+      <c r="S35" s="31"/>
+      <c r="T35" s="31"/>
+      <c r="U35" s="31"/>
+      <c r="V35" s="31"/>
+      <c r="W35" s="31"/>
+      <c r="X35" s="31"/>
+      <c r="Y35" s="31"/>
+      <c r="Z35" s="31"/>
+      <c r="AA35" s="31"/>
+      <c r="AB35" s="31"/>
+      <c r="AC35" s="31"/>
+      <c r="AD35" s="31"/>
+      <c r="AE35" s="31"/>
+      <c r="AF35" s="31"/>
+      <c r="AG35" s="31"/>
+      <c r="AH35" s="31"/>
+      <c r="AI35" s="31"/>
+      <c r="AJ35" s="31"/>
+      <c r="AK35" s="31"/>
+      <c r="AL35" s="31"/>
+      <c r="AM35" s="31"/>
+      <c r="AN35" s="31"/>
+      <c r="AO35" s="31"/>
+      <c r="AP35" s="31"/>
+      <c r="AQ35" s="31"/>
+      <c r="AR35" s="31"/>
+      <c r="AS35" s="31"/>
+      <c r="AT35" s="31"/>
+      <c r="AU35" s="31"/>
+      <c r="AV35" s="31"/>
+      <c r="AW35" s="31"/>
+      <c r="AX35" s="31"/>
+      <c r="AY35" s="31"/>
+      <c r="AZ35" s="31"/>
+      <c r="BA35" s="31"/>
+      <c r="BB35" s="31"/>
+      <c r="BC35" s="31"/>
+      <c r="BD35" s="31"/>
+      <c r="BE35" s="31"/>
+      <c r="BF35" s="31"/>
+      <c r="BG35" s="31"/>
+      <c r="BH35" s="31"/>
+      <c r="BI35" s="31"/>
+      <c r="BJ35" s="31"/>
+      <c r="BK35" s="31"/>
+      <c r="BL35" s="31"/>
+    </row>
+    <row r="36" spans="1:64" s="3" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="45"/>
+      <c r="B36" s="63"/>
+      <c r="C36" s="57"/>
+      <c r="D36" s="23"/>
+      <c r="E36" s="83"/>
+      <c r="F36" s="83"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="14" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="I36" s="31"/>
+      <c r="J36" s="31"/>
+      <c r="K36" s="31"/>
+      <c r="L36" s="31"/>
+      <c r="M36" s="31"/>
+      <c r="N36" s="31"/>
+      <c r="O36" s="31"/>
+      <c r="P36" s="31"/>
+      <c r="Q36" s="31"/>
+      <c r="R36" s="31"/>
+      <c r="S36" s="31"/>
+      <c r="T36" s="31"/>
+      <c r="U36" s="31"/>
+      <c r="V36" s="31"/>
+      <c r="W36" s="31"/>
+      <c r="X36" s="31"/>
+      <c r="Y36" s="31"/>
+      <c r="Z36" s="31"/>
+      <c r="AA36" s="31"/>
+      <c r="AB36" s="31"/>
+      <c r="AC36" s="31"/>
+      <c r="AD36" s="31"/>
+      <c r="AE36" s="31"/>
+      <c r="AF36" s="31"/>
+      <c r="AG36" s="31"/>
+      <c r="AH36" s="31"/>
+      <c r="AI36" s="31"/>
+      <c r="AJ36" s="31"/>
+      <c r="AK36" s="31"/>
+      <c r="AL36" s="31"/>
+      <c r="AM36" s="31"/>
+      <c r="AN36" s="31"/>
+      <c r="AO36" s="31"/>
+      <c r="AP36" s="31"/>
+      <c r="AQ36" s="31"/>
+      <c r="AR36" s="31"/>
+      <c r="AS36" s="31"/>
+      <c r="AT36" s="31"/>
+      <c r="AU36" s="31"/>
+      <c r="AV36" s="31"/>
+      <c r="AW36" s="31"/>
+      <c r="AX36" s="31"/>
+      <c r="AY36" s="31"/>
+      <c r="AZ36" s="31"/>
+      <c r="BA36" s="31"/>
+      <c r="BB36" s="31"/>
+      <c r="BC36" s="31"/>
+      <c r="BD36" s="31"/>
+      <c r="BE36" s="31"/>
+      <c r="BF36" s="31"/>
+      <c r="BG36" s="31"/>
+      <c r="BH36" s="31"/>
+      <c r="BI36" s="31"/>
+      <c r="BJ36" s="31"/>
+      <c r="BK36" s="31"/>
+      <c r="BL36" s="31"/>
+    </row>
+    <row r="37" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="45" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="C37" s="58"/>
+      <c r="D37" s="25"/>
+      <c r="E37" s="84"/>
+      <c r="F37" s="85"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="14" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="I37" s="31"/>
+      <c r="J37" s="31"/>
+      <c r="K37" s="31"/>
+      <c r="L37" s="31"/>
+      <c r="M37" s="31"/>
+      <c r="N37" s="31"/>
+      <c r="O37" s="31"/>
+      <c r="P37" s="31"/>
+      <c r="Q37" s="31"/>
+      <c r="R37" s="31"/>
+      <c r="S37" s="31"/>
+      <c r="T37" s="31"/>
+      <c r="U37" s="31"/>
+      <c r="V37" s="31"/>
+      <c r="W37" s="31"/>
+      <c r="X37" s="31"/>
+      <c r="Y37" s="31"/>
+      <c r="Z37" s="31"/>
+      <c r="AA37" s="31"/>
+      <c r="AB37" s="31"/>
+      <c r="AC37" s="31"/>
+      <c r="AD37" s="31"/>
+      <c r="AE37" s="31"/>
+      <c r="AF37" s="31"/>
+      <c r="AG37" s="31"/>
+      <c r="AH37" s="31"/>
+      <c r="AI37" s="31"/>
+      <c r="AJ37" s="31"/>
+      <c r="AK37" s="31"/>
+      <c r="AL37" s="31"/>
+      <c r="AM37" s="31"/>
+      <c r="AN37" s="31"/>
+      <c r="AO37" s="31"/>
+      <c r="AP37" s="31"/>
+      <c r="AQ37" s="31"/>
+      <c r="AR37" s="31"/>
+      <c r="AS37" s="31"/>
+      <c r="AT37" s="31"/>
+      <c r="AU37" s="31"/>
+      <c r="AV37" s="31"/>
+      <c r="AW37" s="31"/>
+      <c r="AX37" s="31"/>
+      <c r="AY37" s="31"/>
+      <c r="AZ37" s="31"/>
+      <c r="BA37" s="31"/>
+      <c r="BB37" s="31"/>
+      <c r="BC37" s="31"/>
+      <c r="BD37" s="31"/>
+      <c r="BE37" s="31"/>
+      <c r="BF37" s="31"/>
+      <c r="BG37" s="31"/>
+      <c r="BH37" s="31"/>
+      <c r="BI37" s="31"/>
+      <c r="BJ37" s="31"/>
+      <c r="BK37" s="31"/>
+      <c r="BL37" s="31"/>
+    </row>
+    <row r="38" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="45"/>
+      <c r="B38" s="64" t="s">
+        <v>52</v>
+      </c>
+      <c r="C38" s="59" t="s">
+        <v>51</v>
+      </c>
+      <c r="D38" s="26">
+        <v>0</v>
+      </c>
+      <c r="E38" s="86">
+        <f>Inicio_del_proyecto</f>
+        <v>45857</v>
+      </c>
+      <c r="F38" s="86">
+        <f>E38+7</f>
+        <v>45864</v>
+      </c>
+      <c r="G38" s="14"/>
+      <c r="H38" s="14">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="I38" s="31"/>
+      <c r="J38" s="31"/>
+      <c r="K38" s="31"/>
+      <c r="L38" s="31"/>
+      <c r="M38" s="31"/>
+      <c r="N38" s="31"/>
+      <c r="O38" s="31"/>
+      <c r="P38" s="31"/>
+      <c r="Q38" s="31"/>
+      <c r="R38" s="31"/>
+      <c r="S38" s="31"/>
+      <c r="T38" s="31"/>
+      <c r="U38" s="31"/>
+      <c r="V38" s="31"/>
+      <c r="W38" s="31"/>
+      <c r="X38" s="31"/>
+      <c r="Y38" s="31"/>
+      <c r="Z38" s="31"/>
+      <c r="AA38" s="31"/>
+      <c r="AB38" s="31"/>
+      <c r="AC38" s="31"/>
+      <c r="AD38" s="31"/>
+      <c r="AE38" s="31"/>
+      <c r="AF38" s="31"/>
+      <c r="AG38" s="31"/>
+      <c r="AH38" s="31"/>
+      <c r="AI38" s="31"/>
+      <c r="AJ38" s="31"/>
+      <c r="AK38" s="31"/>
+      <c r="AL38" s="31"/>
+      <c r="AM38" s="31"/>
+      <c r="AN38" s="31"/>
+      <c r="AO38" s="31"/>
+      <c r="AP38" s="31"/>
+      <c r="AQ38" s="31"/>
+      <c r="AR38" s="31"/>
+      <c r="AS38" s="31"/>
+      <c r="AT38" s="31"/>
+      <c r="AU38" s="31"/>
+      <c r="AV38" s="31"/>
+      <c r="AW38" s="31"/>
+      <c r="AX38" s="31"/>
+      <c r="AY38" s="31"/>
+      <c r="AZ38" s="31"/>
+      <c r="BA38" s="31"/>
+      <c r="BB38" s="31"/>
+      <c r="BC38" s="31"/>
+      <c r="BD38" s="31"/>
+      <c r="BE38" s="31"/>
+      <c r="BF38" s="31"/>
+      <c r="BG38" s="31"/>
+      <c r="BH38" s="31"/>
+      <c r="BI38" s="31"/>
+      <c r="BJ38" s="31"/>
+      <c r="BK38" s="31"/>
+      <c r="BL38" s="31"/>
+    </row>
+    <row r="39" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="45"/>
+      <c r="B39" s="64" t="s">
+        <v>69</v>
+      </c>
+      <c r="C39" s="59"/>
+      <c r="D39" s="26">
+        <v>0</v>
+      </c>
+      <c r="E39" s="86">
+        <v>45865</v>
+      </c>
+      <c r="F39" s="86">
+        <v>45868</v>
+      </c>
+      <c r="G39" s="14"/>
+      <c r="H39" s="14">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="I39" s="31"/>
+      <c r="J39" s="31"/>
+      <c r="K39" s="31"/>
+      <c r="L39" s="31"/>
+      <c r="M39" s="31"/>
+      <c r="N39" s="31"/>
+      <c r="O39" s="31"/>
+      <c r="P39" s="31"/>
+      <c r="Q39" s="31"/>
+      <c r="R39" s="31"/>
+      <c r="S39" s="31"/>
+      <c r="T39" s="31"/>
+      <c r="U39" s="31"/>
+      <c r="V39" s="31"/>
+      <c r="W39" s="31"/>
+      <c r="X39" s="31"/>
+      <c r="Y39" s="31"/>
+      <c r="Z39" s="31"/>
+      <c r="AA39" s="31"/>
+      <c r="AB39" s="31"/>
+      <c r="AC39" s="31"/>
+      <c r="AD39" s="31"/>
+      <c r="AE39" s="31"/>
+      <c r="AF39" s="31"/>
+      <c r="AG39" s="31"/>
+      <c r="AH39" s="31"/>
+      <c r="AI39" s="31"/>
+      <c r="AJ39" s="31"/>
+      <c r="AK39" s="31"/>
+      <c r="AL39" s="31"/>
+      <c r="AM39" s="31"/>
+      <c r="AN39" s="31"/>
+      <c r="AO39" s="31"/>
+      <c r="AP39" s="31"/>
+      <c r="AQ39" s="31"/>
+      <c r="AR39" s="31"/>
+      <c r="AS39" s="31"/>
+      <c r="AT39" s="31"/>
+      <c r="AU39" s="31"/>
+      <c r="AV39" s="31"/>
+      <c r="AW39" s="31"/>
+      <c r="AX39" s="31"/>
+      <c r="AY39" s="31"/>
+      <c r="AZ39" s="31"/>
+      <c r="BA39" s="31"/>
+      <c r="BB39" s="31"/>
+      <c r="BC39" s="31"/>
+      <c r="BD39" s="31"/>
+      <c r="BE39" s="31"/>
+      <c r="BF39" s="31"/>
+      <c r="BG39" s="31"/>
+      <c r="BH39" s="31"/>
+      <c r="BI39" s="31"/>
+      <c r="BJ39" s="31"/>
+      <c r="BK39" s="31"/>
+      <c r="BL39" s="31"/>
+    </row>
+    <row r="40" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="45"/>
+      <c r="B40" s="89" t="s">
+        <v>70</v>
+      </c>
+      <c r="C40" s="59"/>
+      <c r="D40" s="26">
+        <v>0</v>
+      </c>
+      <c r="E40" s="86">
+        <v>45869</v>
+      </c>
+      <c r="F40" s="86">
+        <v>45871</v>
+      </c>
+      <c r="G40" s="14"/>
+      <c r="H40" s="14">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="I40" s="31"/>
+      <c r="J40" s="31"/>
+      <c r="K40" s="31"/>
+      <c r="L40" s="31"/>
+      <c r="M40" s="31"/>
+      <c r="N40" s="31"/>
+      <c r="O40" s="31"/>
+      <c r="P40" s="31"/>
+      <c r="Q40" s="31"/>
+      <c r="R40" s="31"/>
+      <c r="S40" s="31"/>
+      <c r="T40" s="31"/>
+      <c r="U40" s="31"/>
+      <c r="V40" s="31"/>
+      <c r="W40" s="31"/>
+      <c r="X40" s="31"/>
+      <c r="Y40" s="31"/>
+      <c r="Z40" s="31"/>
+      <c r="AA40" s="31"/>
+      <c r="AB40" s="31"/>
+      <c r="AC40" s="31"/>
+      <c r="AD40" s="31"/>
+      <c r="AE40" s="31"/>
+      <c r="AF40" s="31"/>
+      <c r="AG40" s="31"/>
+      <c r="AH40" s="31"/>
+      <c r="AI40" s="31"/>
+      <c r="AJ40" s="31"/>
+      <c r="AK40" s="31"/>
+      <c r="AL40" s="31"/>
+      <c r="AM40" s="31"/>
+      <c r="AN40" s="31"/>
+      <c r="AO40" s="31"/>
+      <c r="AP40" s="31"/>
+      <c r="AQ40" s="31"/>
+      <c r="AR40" s="31"/>
+      <c r="AS40" s="31"/>
+      <c r="AT40" s="31"/>
+      <c r="AU40" s="31"/>
+      <c r="AV40" s="31"/>
+      <c r="AW40" s="31"/>
+      <c r="AX40" s="31"/>
+      <c r="AY40" s="31"/>
+      <c r="AZ40" s="31"/>
+      <c r="BA40" s="31"/>
+      <c r="BB40" s="31"/>
+      <c r="BC40" s="31"/>
+      <c r="BD40" s="31"/>
+      <c r="BE40" s="31"/>
+      <c r="BF40" s="31"/>
+      <c r="BG40" s="31"/>
+      <c r="BH40" s="31"/>
+      <c r="BI40" s="31"/>
+      <c r="BJ40" s="31"/>
+      <c r="BK40" s="31"/>
+      <c r="BL40" s="31"/>
+    </row>
+    <row r="41" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="45"/>
+      <c r="B41" s="89" t="s">
+        <v>71</v>
+      </c>
+      <c r="C41" s="59"/>
+      <c r="D41" s="26">
+        <v>0</v>
+      </c>
+      <c r="E41" s="86">
+        <v>45872</v>
+      </c>
+      <c r="F41" s="86">
+        <v>45876</v>
+      </c>
+      <c r="G41" s="14"/>
+      <c r="H41" s="14"/>
+      <c r="I41" s="31"/>
+      <c r="J41" s="31"/>
+      <c r="K41" s="31"/>
+      <c r="L41" s="31"/>
+      <c r="M41" s="31"/>
+      <c r="N41" s="31"/>
+      <c r="O41" s="31"/>
+      <c r="P41" s="31"/>
+      <c r="Q41" s="31"/>
+      <c r="R41" s="31"/>
+      <c r="S41" s="31"/>
+      <c r="T41" s="31"/>
+      <c r="U41" s="31"/>
+      <c r="V41" s="31"/>
+      <c r="W41" s="31"/>
+      <c r="X41" s="31"/>
+      <c r="Y41" s="31"/>
+      <c r="Z41" s="31"/>
+      <c r="AA41" s="31"/>
+      <c r="AB41" s="31"/>
+      <c r="AC41" s="31"/>
+      <c r="AD41" s="31"/>
+      <c r="AE41" s="31"/>
+      <c r="AF41" s="31"/>
+      <c r="AG41" s="31"/>
+      <c r="AH41" s="31"/>
+      <c r="AI41" s="31"/>
+      <c r="AJ41" s="31"/>
+      <c r="AK41" s="31"/>
+      <c r="AL41" s="31"/>
+      <c r="AM41" s="31"/>
+      <c r="AN41" s="31"/>
+      <c r="AO41" s="31"/>
+      <c r="AP41" s="31"/>
+      <c r="AQ41" s="31"/>
+      <c r="AR41" s="31"/>
+      <c r="AS41" s="31"/>
+      <c r="AT41" s="31"/>
+      <c r="AU41" s="31"/>
+      <c r="AV41" s="31"/>
+      <c r="AW41" s="31"/>
+      <c r="AX41" s="31"/>
+      <c r="AY41" s="31"/>
+      <c r="AZ41" s="31"/>
+      <c r="BA41" s="31"/>
+      <c r="BB41" s="31"/>
+      <c r="BC41" s="31"/>
+      <c r="BD41" s="31"/>
+      <c r="BE41" s="31"/>
+      <c r="BF41" s="31"/>
+      <c r="BG41" s="31"/>
+      <c r="BH41" s="31"/>
+      <c r="BI41" s="31"/>
+      <c r="BJ41" s="31"/>
+      <c r="BK41" s="31"/>
+      <c r="BL41" s="31"/>
+    </row>
+    <row r="42" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="45"/>
+      <c r="B42" s="89" t="s">
+        <v>72</v>
+      </c>
+      <c r="C42" s="59"/>
+      <c r="D42" s="26">
+        <v>0</v>
+      </c>
+      <c r="E42" s="86">
+        <v>45877</v>
+      </c>
+      <c r="F42" s="86">
+        <v>45881</v>
+      </c>
+      <c r="G42" s="14"/>
+      <c r="H42" s="14"/>
+      <c r="I42" s="31"/>
+      <c r="J42" s="31"/>
+      <c r="K42" s="31"/>
+      <c r="L42" s="31"/>
+      <c r="M42" s="31"/>
+      <c r="N42" s="31"/>
+      <c r="O42" s="31"/>
+      <c r="P42" s="31"/>
+      <c r="Q42" s="31"/>
+      <c r="R42" s="31"/>
+      <c r="S42" s="31"/>
+      <c r="T42" s="31"/>
+      <c r="U42" s="31"/>
+      <c r="V42" s="31"/>
+      <c r="W42" s="31"/>
+      <c r="X42" s="31"/>
+      <c r="Y42" s="31"/>
+      <c r="Z42" s="31"/>
+      <c r="AA42" s="31"/>
+      <c r="AB42" s="31"/>
+      <c r="AC42" s="31"/>
+      <c r="AD42" s="31"/>
+      <c r="AE42" s="31"/>
+      <c r="AF42" s="31"/>
+      <c r="AG42" s="31"/>
+      <c r="AH42" s="31"/>
+      <c r="AI42" s="31"/>
+      <c r="AJ42" s="31"/>
+      <c r="AK42" s="31"/>
+      <c r="AL42" s="31"/>
+      <c r="AM42" s="31"/>
+      <c r="AN42" s="31"/>
+      <c r="AO42" s="31"/>
+      <c r="AP42" s="31"/>
+      <c r="AQ42" s="31"/>
+      <c r="AR42" s="31"/>
+      <c r="AS42" s="31"/>
+      <c r="AT42" s="31"/>
+      <c r="AU42" s="31"/>
+      <c r="AV42" s="31"/>
+      <c r="AW42" s="31"/>
+      <c r="AX42" s="31"/>
+      <c r="AY42" s="31"/>
+      <c r="AZ42" s="31"/>
+      <c r="BA42" s="31"/>
+      <c r="BB42" s="31"/>
+      <c r="BC42" s="31"/>
+      <c r="BD42" s="31"/>
+      <c r="BE42" s="31"/>
+      <c r="BF42" s="31"/>
+      <c r="BG42" s="31"/>
+      <c r="BH42" s="31"/>
+      <c r="BI42" s="31"/>
+      <c r="BJ42" s="31"/>
+      <c r="BK42" s="31"/>
+      <c r="BL42" s="31"/>
+    </row>
+    <row r="43" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="45"/>
+      <c r="B43" s="89" t="s">
+        <v>73</v>
+      </c>
+      <c r="C43" s="59"/>
+      <c r="D43" s="26">
+        <v>0</v>
+      </c>
+      <c r="E43" s="86">
+        <v>45869</v>
+      </c>
+      <c r="F43" s="86">
+        <v>45878</v>
+      </c>
+      <c r="G43" s="14"/>
+      <c r="H43" s="14"/>
+      <c r="I43" s="31"/>
+      <c r="J43" s="31"/>
+      <c r="K43" s="31"/>
+      <c r="L43" s="31"/>
+      <c r="M43" s="31"/>
+      <c r="N43" s="31"/>
+      <c r="O43" s="31"/>
+      <c r="P43" s="31"/>
+      <c r="Q43" s="31"/>
+      <c r="R43" s="31"/>
+      <c r="S43" s="31"/>
+      <c r="T43" s="31"/>
+      <c r="U43" s="31"/>
+      <c r="V43" s="31"/>
+      <c r="W43" s="31"/>
+      <c r="X43" s="31"/>
+      <c r="Y43" s="31"/>
+      <c r="Z43" s="31"/>
+      <c r="AA43" s="31"/>
+      <c r="AB43" s="31"/>
+      <c r="AC43" s="31"/>
+      <c r="AD43" s="31"/>
+      <c r="AE43" s="31"/>
+      <c r="AF43" s="31"/>
+      <c r="AG43" s="31"/>
+      <c r="AH43" s="31"/>
+      <c r="AI43" s="31"/>
+      <c r="AJ43" s="31"/>
+      <c r="AK43" s="31"/>
+      <c r="AL43" s="31"/>
+      <c r="AM43" s="31"/>
+      <c r="AN43" s="31"/>
+      <c r="AO43" s="31"/>
+      <c r="AP43" s="31"/>
+      <c r="AQ43" s="31"/>
+      <c r="AR43" s="31"/>
+      <c r="AS43" s="31"/>
+      <c r="AT43" s="31"/>
+      <c r="AU43" s="31"/>
+      <c r="AV43" s="31"/>
+      <c r="AW43" s="31"/>
+      <c r="AX43" s="31"/>
+      <c r="AY43" s="31"/>
+      <c r="AZ43" s="31"/>
+      <c r="BA43" s="31"/>
+      <c r="BB43" s="31"/>
+      <c r="BC43" s="31"/>
+      <c r="BD43" s="31"/>
+      <c r="BE43" s="31"/>
+      <c r="BF43" s="31"/>
+      <c r="BG43" s="31"/>
+      <c r="BH43" s="31"/>
+      <c r="BI43" s="31"/>
+      <c r="BJ43" s="31"/>
+      <c r="BK43" s="31"/>
+      <c r="BL43" s="31"/>
+    </row>
+    <row r="44" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="45"/>
+      <c r="B44" s="89" t="s">
+        <v>74</v>
+      </c>
+      <c r="C44" s="59"/>
+      <c r="D44" s="26">
+        <v>0</v>
+      </c>
+      <c r="E44" s="86">
+        <v>45872</v>
+      </c>
+      <c r="F44" s="86">
+        <v>45881</v>
+      </c>
+      <c r="G44" s="14"/>
+      <c r="H44" s="14"/>
+      <c r="I44" s="31"/>
+      <c r="J44" s="31"/>
+      <c r="K44" s="31"/>
+      <c r="L44" s="31"/>
+      <c r="M44" s="31"/>
+      <c r="N44" s="31"/>
+      <c r="O44" s="31"/>
+      <c r="P44" s="31"/>
+      <c r="Q44" s="31"/>
+      <c r="R44" s="31"/>
+      <c r="S44" s="31"/>
+      <c r="T44" s="31"/>
+      <c r="U44" s="31"/>
+      <c r="V44" s="31"/>
+      <c r="W44" s="31"/>
+      <c r="X44" s="31"/>
+      <c r="Y44" s="31"/>
+      <c r="Z44" s="31"/>
+      <c r="AA44" s="31"/>
+      <c r="AB44" s="31"/>
+      <c r="AC44" s="31"/>
+      <c r="AD44" s="31"/>
+      <c r="AE44" s="31"/>
+      <c r="AF44" s="31"/>
+      <c r="AG44" s="31"/>
+      <c r="AH44" s="31"/>
+      <c r="AI44" s="31"/>
+      <c r="AJ44" s="31"/>
+      <c r="AK44" s="31"/>
+      <c r="AL44" s="31"/>
+      <c r="AM44" s="31"/>
+      <c r="AN44" s="31"/>
+      <c r="AO44" s="31"/>
+      <c r="AP44" s="31"/>
+      <c r="AQ44" s="31"/>
+      <c r="AR44" s="31"/>
+      <c r="AS44" s="31"/>
+      <c r="AT44" s="31"/>
+      <c r="AU44" s="31"/>
+      <c r="AV44" s="31"/>
+      <c r="AW44" s="31"/>
+      <c r="AX44" s="31"/>
+      <c r="AY44" s="31"/>
+      <c r="AZ44" s="31"/>
+      <c r="BA44" s="31"/>
+      <c r="BB44" s="31"/>
+      <c r="BC44" s="31"/>
+      <c r="BD44" s="31"/>
+      <c r="BE44" s="31"/>
+      <c r="BF44" s="31"/>
+      <c r="BG44" s="31"/>
+      <c r="BH44" s="31"/>
+      <c r="BI44" s="31"/>
+      <c r="BJ44" s="31"/>
+      <c r="BK44" s="31"/>
+      <c r="BL44" s="31"/>
+    </row>
+    <row r="45" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="45"/>
+      <c r="B45" s="89" t="s">
+        <v>75</v>
+      </c>
+      <c r="C45" s="59"/>
+      <c r="D45" s="26">
+        <v>0</v>
+      </c>
+      <c r="E45" s="86">
+        <v>45877</v>
+      </c>
+      <c r="F45" s="86">
+        <v>45881</v>
+      </c>
+      <c r="G45" s="14"/>
+      <c r="H45" s="14"/>
+      <c r="I45" s="31"/>
+      <c r="J45" s="31"/>
+      <c r="K45" s="31"/>
+      <c r="L45" s="31"/>
+      <c r="M45" s="31"/>
+      <c r="N45" s="31"/>
+      <c r="O45" s="31"/>
+      <c r="P45" s="31"/>
+      <c r="Q45" s="31"/>
+      <c r="R45" s="31"/>
+      <c r="S45" s="31"/>
+      <c r="T45" s="31"/>
+      <c r="U45" s="31"/>
+      <c r="V45" s="31"/>
+      <c r="W45" s="31"/>
+      <c r="X45" s="31"/>
+      <c r="Y45" s="31"/>
+      <c r="Z45" s="31"/>
+      <c r="AA45" s="31"/>
+      <c r="AB45" s="31"/>
+      <c r="AC45" s="31"/>
+      <c r="AD45" s="31"/>
+      <c r="AE45" s="31"/>
+      <c r="AF45" s="31"/>
+      <c r="AG45" s="31"/>
+      <c r="AH45" s="31"/>
+      <c r="AI45" s="31"/>
+      <c r="AJ45" s="31"/>
+      <c r="AK45" s="31"/>
+      <c r="AL45" s="31"/>
+      <c r="AM45" s="31"/>
+      <c r="AN45" s="31"/>
+      <c r="AO45" s="31"/>
+      <c r="AP45" s="31"/>
+      <c r="AQ45" s="31"/>
+      <c r="AR45" s="31"/>
+      <c r="AS45" s="31"/>
+      <c r="AT45" s="31"/>
+      <c r="AU45" s="31"/>
+      <c r="AV45" s="31"/>
+      <c r="AW45" s="31"/>
+      <c r="AX45" s="31"/>
+      <c r="AY45" s="31"/>
+      <c r="AZ45" s="31"/>
+      <c r="BA45" s="31"/>
+      <c r="BB45" s="31"/>
+      <c r="BC45" s="31"/>
+      <c r="BD45" s="31"/>
+      <c r="BE45" s="31"/>
+      <c r="BF45" s="31"/>
+      <c r="BG45" s="31"/>
+      <c r="BH45" s="31"/>
+      <c r="BI45" s="31"/>
+      <c r="BJ45" s="31"/>
+      <c r="BK45" s="31"/>
+      <c r="BL45" s="31"/>
+    </row>
+    <row r="46" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="45"/>
+      <c r="B46" s="89" t="s">
+        <v>76</v>
+      </c>
+      <c r="C46" s="59"/>
+      <c r="D46" s="26">
+        <v>0</v>
+      </c>
+      <c r="E46" s="86">
+        <v>45882</v>
+      </c>
+      <c r="F46" s="86">
+        <v>45886</v>
+      </c>
+      <c r="G46" s="14"/>
+      <c r="H46" s="14"/>
+      <c r="I46" s="31"/>
+      <c r="J46" s="31"/>
+      <c r="K46" s="31"/>
+      <c r="L46" s="31"/>
+      <c r="M46" s="31"/>
+      <c r="N46" s="31"/>
+      <c r="O46" s="31"/>
+      <c r="P46" s="31"/>
+      <c r="Q46" s="31"/>
+      <c r="R46" s="31"/>
+      <c r="S46" s="31"/>
+      <c r="T46" s="31"/>
+      <c r="U46" s="31"/>
+      <c r="V46" s="31"/>
+      <c r="W46" s="31"/>
+      <c r="X46" s="31"/>
+      <c r="Y46" s="31"/>
+      <c r="Z46" s="31"/>
+      <c r="AA46" s="31"/>
+      <c r="AB46" s="31"/>
+      <c r="AC46" s="31"/>
+      <c r="AD46" s="31"/>
+      <c r="AE46" s="31"/>
+      <c r="AF46" s="31"/>
+      <c r="AG46" s="31"/>
+      <c r="AH46" s="31"/>
+      <c r="AI46" s="31"/>
+      <c r="AJ46" s="31"/>
+      <c r="AK46" s="31"/>
+      <c r="AL46" s="31"/>
+      <c r="AM46" s="31"/>
+      <c r="AN46" s="31"/>
+      <c r="AO46" s="31"/>
+      <c r="AP46" s="31"/>
+      <c r="AQ46" s="31"/>
+      <c r="AR46" s="31"/>
+      <c r="AS46" s="31"/>
+      <c r="AT46" s="31"/>
+      <c r="AU46" s="31"/>
+      <c r="AV46" s="31"/>
+      <c r="AW46" s="31"/>
+      <c r="AX46" s="31"/>
+      <c r="AY46" s="31"/>
+      <c r="AZ46" s="31"/>
+      <c r="BA46" s="31"/>
+      <c r="BB46" s="31"/>
+      <c r="BC46" s="31"/>
+      <c r="BD46" s="31"/>
+      <c r="BE46" s="31"/>
+      <c r="BF46" s="31"/>
+      <c r="BG46" s="31"/>
+      <c r="BH46" s="31"/>
+      <c r="BI46" s="31"/>
+      <c r="BJ46" s="31"/>
+      <c r="BK46" s="31"/>
+      <c r="BL46" s="31"/>
+    </row>
+    <row r="47" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="45"/>
+      <c r="B47" s="89" t="s">
+        <v>77</v>
+      </c>
+      <c r="C47" s="59"/>
+      <c r="D47" s="26">
+        <v>0</v>
+      </c>
+      <c r="E47" s="86">
+        <v>45887</v>
+      </c>
+      <c r="F47" s="86">
+        <v>45891</v>
+      </c>
+      <c r="G47" s="14"/>
+      <c r="H47" s="14"/>
+      <c r="I47" s="31"/>
+      <c r="J47" s="31"/>
+      <c r="K47" s="31"/>
+      <c r="L47" s="31"/>
+      <c r="M47" s="31"/>
+      <c r="N47" s="31"/>
+      <c r="O47" s="31"/>
+      <c r="P47" s="31"/>
+      <c r="Q47" s="31"/>
+      <c r="R47" s="31"/>
+      <c r="S47" s="31"/>
+      <c r="T47" s="31"/>
+      <c r="U47" s="31"/>
+      <c r="V47" s="31"/>
+      <c r="W47" s="31"/>
+      <c r="X47" s="31"/>
+      <c r="Y47" s="31"/>
+      <c r="Z47" s="31"/>
+      <c r="AA47" s="31"/>
+      <c r="AB47" s="31"/>
+      <c r="AC47" s="31"/>
+      <c r="AD47" s="31"/>
+      <c r="AE47" s="31"/>
+      <c r="AF47" s="31"/>
+      <c r="AG47" s="31"/>
+      <c r="AH47" s="31"/>
+      <c r="AI47" s="31"/>
+      <c r="AJ47" s="31"/>
+      <c r="AK47" s="31"/>
+      <c r="AL47" s="31"/>
+      <c r="AM47" s="31"/>
+      <c r="AN47" s="31"/>
+      <c r="AO47" s="31"/>
+      <c r="AP47" s="31"/>
+      <c r="AQ47" s="31"/>
+      <c r="AR47" s="31"/>
+      <c r="AS47" s="31"/>
+      <c r="AT47" s="31"/>
+      <c r="AU47" s="31"/>
+      <c r="AV47" s="31"/>
+      <c r="AW47" s="31"/>
+      <c r="AX47" s="31"/>
+      <c r="AY47" s="31"/>
+      <c r="AZ47" s="31"/>
+      <c r="BA47" s="31"/>
+      <c r="BB47" s="31"/>
+      <c r="BC47" s="31"/>
+      <c r="BD47" s="31"/>
+      <c r="BE47" s="31"/>
+      <c r="BF47" s="31"/>
+      <c r="BG47" s="31"/>
+      <c r="BH47" s="31"/>
+      <c r="BI47" s="31"/>
+      <c r="BJ47" s="31"/>
+      <c r="BK47" s="31"/>
+      <c r="BL47" s="31"/>
+    </row>
+    <row r="48" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="45"/>
+      <c r="B48" s="89" t="s">
+        <v>78</v>
+      </c>
+      <c r="C48" s="59"/>
+      <c r="D48" s="26">
+        <v>0</v>
+      </c>
+      <c r="E48" s="86">
+        <v>45892</v>
+      </c>
+      <c r="F48" s="86">
+        <v>45895</v>
+      </c>
+      <c r="G48" s="14"/>
+      <c r="H48" s="14"/>
+      <c r="I48" s="31"/>
+      <c r="J48" s="31"/>
+      <c r="K48" s="31"/>
+      <c r="L48" s="31"/>
+      <c r="M48" s="31"/>
+      <c r="N48" s="31"/>
+      <c r="O48" s="31"/>
+      <c r="P48" s="31"/>
+      <c r="Q48" s="31"/>
+      <c r="R48" s="31"/>
+      <c r="S48" s="31"/>
+      <c r="T48" s="31"/>
+      <c r="U48" s="31"/>
+      <c r="V48" s="31"/>
+      <c r="W48" s="31"/>
+      <c r="X48" s="31"/>
+      <c r="Y48" s="31"/>
+      <c r="Z48" s="31"/>
+      <c r="AA48" s="31"/>
+      <c r="AB48" s="31"/>
+      <c r="AC48" s="31"/>
+      <c r="AD48" s="31"/>
+      <c r="AE48" s="31"/>
+      <c r="AF48" s="31"/>
+      <c r="AG48" s="31"/>
+      <c r="AH48" s="31"/>
+      <c r="AI48" s="31"/>
+      <c r="AJ48" s="31"/>
+      <c r="AK48" s="31"/>
+      <c r="AL48" s="31"/>
+      <c r="AM48" s="31"/>
+      <c r="AN48" s="31"/>
+      <c r="AO48" s="31"/>
+      <c r="AP48" s="31"/>
+      <c r="AQ48" s="31"/>
+      <c r="AR48" s="31"/>
+      <c r="AS48" s="31"/>
+      <c r="AT48" s="31"/>
+      <c r="AU48" s="31"/>
+      <c r="AV48" s="31"/>
+      <c r="AW48" s="31"/>
+      <c r="AX48" s="31"/>
+      <c r="AY48" s="31"/>
+      <c r="AZ48" s="31"/>
+      <c r="BA48" s="31"/>
+      <c r="BB48" s="31"/>
+      <c r="BC48" s="31"/>
+      <c r="BD48" s="31"/>
+      <c r="BE48" s="31"/>
+      <c r="BF48" s="31"/>
+      <c r="BG48" s="31"/>
+      <c r="BH48" s="31"/>
+      <c r="BI48" s="31"/>
+      <c r="BJ48" s="31"/>
+      <c r="BK48" s="31"/>
+      <c r="BL48" s="31"/>
+    </row>
+    <row r="49" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="45"/>
+      <c r="B49" s="89" t="s">
+        <v>79</v>
+      </c>
+      <c r="C49" s="59"/>
+      <c r="D49" s="26">
+        <v>0</v>
+      </c>
+      <c r="E49" s="86">
+        <v>45896</v>
+      </c>
+      <c r="F49" s="86">
+        <v>45899</v>
+      </c>
+      <c r="G49" s="14"/>
+      <c r="H49" s="14"/>
+      <c r="I49" s="31"/>
+      <c r="J49" s="31"/>
+      <c r="K49" s="31"/>
+      <c r="L49" s="31"/>
+      <c r="M49" s="31"/>
+      <c r="N49" s="31"/>
+      <c r="O49" s="31"/>
+      <c r="P49" s="31"/>
+      <c r="Q49" s="31"/>
+      <c r="R49" s="31"/>
+      <c r="S49" s="31"/>
+      <c r="T49" s="31"/>
+      <c r="U49" s="31"/>
+      <c r="V49" s="31"/>
+      <c r="W49" s="31"/>
+      <c r="X49" s="31"/>
+      <c r="Y49" s="31"/>
+      <c r="Z49" s="31"/>
+      <c r="AA49" s="31"/>
+      <c r="AB49" s="31"/>
+      <c r="AC49" s="31"/>
+      <c r="AD49" s="31"/>
+      <c r="AE49" s="31"/>
+      <c r="AF49" s="31"/>
+      <c r="AG49" s="31"/>
+      <c r="AH49" s="31"/>
+      <c r="AI49" s="31"/>
+      <c r="AJ49" s="31"/>
+      <c r="AK49" s="31"/>
+      <c r="AL49" s="31"/>
+      <c r="AM49" s="31"/>
+      <c r="AN49" s="31"/>
+      <c r="AO49" s="31"/>
+      <c r="AP49" s="31"/>
+      <c r="AQ49" s="31"/>
+      <c r="AR49" s="31"/>
+      <c r="AS49" s="31"/>
+      <c r="AT49" s="31"/>
+      <c r="AU49" s="31"/>
+      <c r="AV49" s="31"/>
+      <c r="AW49" s="31"/>
+      <c r="AX49" s="31"/>
+      <c r="AY49" s="31"/>
+      <c r="AZ49" s="31"/>
+      <c r="BA49" s="31"/>
+      <c r="BB49" s="31"/>
+      <c r="BC49" s="31"/>
+      <c r="BD49" s="31"/>
+      <c r="BE49" s="31"/>
+      <c r="BF49" s="31"/>
+      <c r="BG49" s="31"/>
+      <c r="BH49" s="31"/>
+      <c r="BI49" s="31"/>
+      <c r="BJ49" s="31"/>
+      <c r="BK49" s="31"/>
+      <c r="BL49" s="31"/>
+    </row>
+    <row r="50" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="45"/>
+      <c r="B50" s="89" t="s">
+        <v>80</v>
+      </c>
+      <c r="C50" s="59"/>
+      <c r="D50" s="26">
+        <v>0</v>
+      </c>
+      <c r="E50" s="86">
+        <v>45900</v>
+      </c>
+      <c r="F50" s="86">
+        <v>45903</v>
+      </c>
+      <c r="G50" s="14"/>
+      <c r="H50" s="14"/>
+      <c r="I50" s="31"/>
+      <c r="J50" s="31"/>
+      <c r="K50" s="31"/>
+      <c r="L50" s="31"/>
+      <c r="M50" s="31"/>
+      <c r="N50" s="31"/>
+      <c r="O50" s="31"/>
+      <c r="P50" s="31"/>
+      <c r="Q50" s="31"/>
+      <c r="R50" s="31"/>
+      <c r="S50" s="31"/>
+      <c r="T50" s="31"/>
+      <c r="U50" s="31"/>
+      <c r="V50" s="31"/>
+      <c r="W50" s="31"/>
+      <c r="X50" s="31"/>
+      <c r="Y50" s="31"/>
+      <c r="Z50" s="31"/>
+      <c r="AA50" s="31"/>
+      <c r="AB50" s="31"/>
+      <c r="AC50" s="31"/>
+      <c r="AD50" s="31"/>
+      <c r="AE50" s="31"/>
+      <c r="AF50" s="31"/>
+      <c r="AG50" s="31"/>
+      <c r="AH50" s="31"/>
+      <c r="AI50" s="31"/>
+      <c r="AJ50" s="31"/>
+      <c r="AK50" s="31"/>
+      <c r="AL50" s="31"/>
+      <c r="AM50" s="31"/>
+      <c r="AN50" s="31"/>
+      <c r="AO50" s="31"/>
+      <c r="AP50" s="31"/>
+      <c r="AQ50" s="31"/>
+      <c r="AR50" s="31"/>
+      <c r="AS50" s="31"/>
+      <c r="AT50" s="31"/>
+      <c r="AU50" s="31"/>
+      <c r="AV50" s="31"/>
+      <c r="AW50" s="31"/>
+      <c r="AX50" s="31"/>
+      <c r="AY50" s="31"/>
+      <c r="AZ50" s="31"/>
+      <c r="BA50" s="31"/>
+      <c r="BB50" s="31"/>
+      <c r="BC50" s="31"/>
+      <c r="BD50" s="31"/>
+      <c r="BE50" s="31"/>
+      <c r="BF50" s="31"/>
+      <c r="BG50" s="31"/>
+      <c r="BH50" s="31"/>
+      <c r="BI50" s="31"/>
+      <c r="BJ50" s="31"/>
+      <c r="BK50" s="31"/>
+      <c r="BL50" s="31"/>
+    </row>
+    <row r="51" spans="1:64" s="3" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="45"/>
+      <c r="B51" s="89"/>
+      <c r="C51" s="59"/>
+      <c r="D51" s="26"/>
+      <c r="E51" s="86"/>
+      <c r="F51" s="86"/>
+      <c r="G51" s="14"/>
+      <c r="H51" s="14"/>
+      <c r="I51" s="31"/>
+      <c r="J51" s="31"/>
+      <c r="K51" s="31"/>
+      <c r="L51" s="31"/>
+      <c r="M51" s="31"/>
+      <c r="N51" s="31"/>
+      <c r="O51" s="31"/>
+      <c r="P51" s="31"/>
+      <c r="Q51" s="31"/>
+      <c r="R51" s="31"/>
+      <c r="S51" s="31"/>
+      <c r="T51" s="31"/>
+      <c r="U51" s="31"/>
+      <c r="V51" s="31"/>
+      <c r="W51" s="31"/>
+      <c r="X51" s="31"/>
+      <c r="Y51" s="31"/>
+      <c r="Z51" s="31"/>
+      <c r="AA51" s="31"/>
+      <c r="AB51" s="31"/>
+      <c r="AC51" s="31"/>
+      <c r="AD51" s="31"/>
+      <c r="AE51" s="31"/>
+      <c r="AF51" s="31"/>
+      <c r="AG51" s="31"/>
+      <c r="AH51" s="31"/>
+      <c r="AI51" s="31"/>
+      <c r="AJ51" s="31"/>
+      <c r="AK51" s="31"/>
+      <c r="AL51" s="31"/>
+      <c r="AM51" s="31"/>
+      <c r="AN51" s="31"/>
+      <c r="AO51" s="31"/>
+      <c r="AP51" s="31"/>
+      <c r="AQ51" s="31"/>
+      <c r="AR51" s="31"/>
+      <c r="AS51" s="31"/>
+      <c r="AT51" s="31"/>
+      <c r="AU51" s="31"/>
+      <c r="AV51" s="31"/>
+      <c r="AW51" s="31"/>
+      <c r="AX51" s="31"/>
+      <c r="AY51" s="31"/>
+      <c r="AZ51" s="31"/>
+      <c r="BA51" s="31"/>
+      <c r="BB51" s="31"/>
+      <c r="BC51" s="31"/>
+      <c r="BD51" s="31"/>
+      <c r="BE51" s="31"/>
+      <c r="BF51" s="31"/>
+      <c r="BG51" s="31"/>
+      <c r="BH51" s="31"/>
+      <c r="BI51" s="31"/>
+      <c r="BJ51" s="31"/>
+      <c r="BK51" s="31"/>
+      <c r="BL51" s="31"/>
+    </row>
+    <row r="52" spans="1:64" s="3" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="45"/>
+      <c r="B52" s="89"/>
+      <c r="C52" s="59"/>
+      <c r="D52" s="26"/>
+      <c r="E52" s="86"/>
+      <c r="F52" s="86"/>
+      <c r="G52" s="14"/>
+      <c r="H52" s="14"/>
+      <c r="I52" s="31"/>
+      <c r="J52" s="31"/>
+      <c r="K52" s="31"/>
+      <c r="L52" s="31"/>
+      <c r="M52" s="31"/>
+      <c r="N52" s="31"/>
+      <c r="O52" s="31"/>
+      <c r="P52" s="31"/>
+      <c r="Q52" s="31"/>
+      <c r="R52" s="31"/>
+      <c r="S52" s="31"/>
+      <c r="T52" s="31"/>
+      <c r="U52" s="31"/>
+      <c r="V52" s="31"/>
+      <c r="W52" s="31"/>
+      <c r="X52" s="31"/>
+      <c r="Y52" s="31"/>
+      <c r="Z52" s="31"/>
+      <c r="AA52" s="31"/>
+      <c r="AB52" s="31"/>
+      <c r="AC52" s="31"/>
+      <c r="AD52" s="31"/>
+      <c r="AE52" s="31"/>
+      <c r="AF52" s="31"/>
+      <c r="AG52" s="31"/>
+      <c r="AH52" s="31"/>
+      <c r="AI52" s="31"/>
+      <c r="AJ52" s="31"/>
+      <c r="AK52" s="31"/>
+      <c r="AL52" s="31"/>
+      <c r="AM52" s="31"/>
+      <c r="AN52" s="31"/>
+      <c r="AO52" s="31"/>
+      <c r="AP52" s="31"/>
+      <c r="AQ52" s="31"/>
+      <c r="AR52" s="31"/>
+      <c r="AS52" s="31"/>
+      <c r="AT52" s="31"/>
+      <c r="AU52" s="31"/>
+      <c r="AV52" s="31"/>
+      <c r="AW52" s="31"/>
+      <c r="AX52" s="31"/>
+      <c r="AY52" s="31"/>
+      <c r="AZ52" s="31"/>
+      <c r="BA52" s="31"/>
+      <c r="BB52" s="31"/>
+      <c r="BC52" s="31"/>
+      <c r="BD52" s="31"/>
+      <c r="BE52" s="31"/>
+      <c r="BF52" s="31"/>
+      <c r="BG52" s="31"/>
+      <c r="BH52" s="31"/>
+      <c r="BI52" s="31"/>
+      <c r="BJ52" s="31"/>
+      <c r="BK52" s="31"/>
+      <c r="BL52" s="31"/>
+    </row>
+    <row r="53" spans="1:64" s="3" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="45"/>
+      <c r="B53" s="64"/>
+      <c r="C53" s="59"/>
+      <c r="D53" s="26"/>
+      <c r="E53" s="86"/>
+      <c r="F53" s="86"/>
+      <c r="G53" s="14"/>
+      <c r="H53" s="14" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="I53" s="31"/>
+      <c r="J53" s="31"/>
+      <c r="K53" s="31"/>
+      <c r="L53" s="31"/>
+      <c r="M53" s="31"/>
+      <c r="N53" s="31"/>
+      <c r="O53" s="31"/>
+      <c r="P53" s="31"/>
+      <c r="Q53" s="31"/>
+      <c r="R53" s="31"/>
+      <c r="S53" s="31"/>
+      <c r="T53" s="31"/>
+      <c r="U53" s="31"/>
+      <c r="V53" s="31"/>
+      <c r="W53" s="31"/>
+      <c r="X53" s="31"/>
+      <c r="Y53" s="31"/>
+      <c r="Z53" s="31"/>
+      <c r="AA53" s="31"/>
+      <c r="AB53" s="31"/>
+      <c r="AC53" s="31"/>
+      <c r="AD53" s="31"/>
+      <c r="AE53" s="31"/>
+      <c r="AF53" s="31"/>
+      <c r="AG53" s="31"/>
+      <c r="AH53" s="31"/>
+      <c r="AI53" s="31"/>
+      <c r="AJ53" s="31"/>
+      <c r="AK53" s="31"/>
+      <c r="AL53" s="31"/>
+      <c r="AM53" s="31"/>
+      <c r="AN53" s="31"/>
+      <c r="AO53" s="31"/>
+      <c r="AP53" s="31"/>
+      <c r="AQ53" s="31"/>
+      <c r="AR53" s="31"/>
+      <c r="AS53" s="31"/>
+      <c r="AT53" s="31"/>
+      <c r="AU53" s="31"/>
+      <c r="AV53" s="31"/>
+      <c r="AW53" s="31"/>
+      <c r="AX53" s="31"/>
+      <c r="AY53" s="31"/>
+      <c r="AZ53" s="31"/>
+      <c r="BA53" s="31"/>
+      <c r="BB53" s="31"/>
+      <c r="BC53" s="31"/>
+      <c r="BD53" s="31"/>
+      <c r="BE53" s="31"/>
+      <c r="BF53" s="31"/>
+      <c r="BG53" s="31"/>
+      <c r="BH53" s="31"/>
+      <c r="BI53" s="31"/>
+      <c r="BJ53" s="31"/>
+      <c r="BK53" s="31"/>
+      <c r="BL53" s="31"/>
+    </row>
+    <row r="54" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="45"/>
+      <c r="B54" s="64" t="s">
+        <v>57</v>
+      </c>
+      <c r="C54" s="59"/>
+      <c r="D54" s="26"/>
+      <c r="E54" s="86"/>
+      <c r="F54" s="86"/>
+      <c r="G54" s="14"/>
+      <c r="H54" s="14" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="I54" s="31"/>
+      <c r="J54" s="31"/>
+      <c r="K54" s="31"/>
+      <c r="L54" s="31"/>
+      <c r="M54" s="31"/>
+      <c r="N54" s="31"/>
+      <c r="O54" s="31"/>
+      <c r="P54" s="31"/>
+      <c r="Q54" s="31"/>
+      <c r="R54" s="31"/>
+      <c r="S54" s="31"/>
+      <c r="T54" s="31"/>
+      <c r="U54" s="31"/>
+      <c r="V54" s="31"/>
+      <c r="W54" s="31"/>
+      <c r="X54" s="31"/>
+      <c r="Y54" s="31"/>
+      <c r="Z54" s="31"/>
+      <c r="AA54" s="31"/>
+      <c r="AB54" s="31"/>
+      <c r="AC54" s="31"/>
+      <c r="AD54" s="31"/>
+      <c r="AE54" s="31"/>
+      <c r="AF54" s="31"/>
+      <c r="AG54" s="31"/>
+      <c r="AH54" s="31"/>
+      <c r="AI54" s="31"/>
+      <c r="AJ54" s="31"/>
+      <c r="AK54" s="31"/>
+      <c r="AL54" s="31"/>
+      <c r="AM54" s="31"/>
+      <c r="AN54" s="31"/>
+      <c r="AO54" s="31"/>
+      <c r="AP54" s="31"/>
+      <c r="AQ54" s="31"/>
+      <c r="AR54" s="31"/>
+      <c r="AS54" s="31"/>
+      <c r="AT54" s="31"/>
+      <c r="AU54" s="31"/>
+      <c r="AV54" s="31"/>
+      <c r="AW54" s="31"/>
+      <c r="AX54" s="31"/>
+      <c r="AY54" s="31"/>
+      <c r="AZ54" s="31"/>
+      <c r="BA54" s="31"/>
+      <c r="BB54" s="31"/>
+      <c r="BC54" s="31"/>
+      <c r="BD54" s="31"/>
+      <c r="BE54" s="31"/>
+      <c r="BF54" s="31"/>
+      <c r="BG54" s="31"/>
+      <c r="BH54" s="31"/>
+      <c r="BI54" s="31"/>
+      <c r="BJ54" s="31"/>
+      <c r="BK54" s="31"/>
+      <c r="BL54" s="31"/>
+    </row>
+    <row r="55" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="45" t="s">
+        <v>12</v>
+      </c>
+      <c r="B55" s="65"/>
+      <c r="C55" s="60"/>
+      <c r="D55" s="13"/>
+      <c r="E55" s="87"/>
+      <c r="F55" s="87"/>
+      <c r="G55" s="14"/>
+      <c r="H55" s="14" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="I55" s="31"/>
+      <c r="J55" s="31"/>
+      <c r="K55" s="31"/>
+      <c r="L55" s="31"/>
+      <c r="M55" s="31"/>
+      <c r="N55" s="31"/>
+      <c r="O55" s="31"/>
+      <c r="P55" s="31"/>
+      <c r="Q55" s="31"/>
+      <c r="R55" s="31"/>
+      <c r="S55" s="31"/>
+      <c r="T55" s="31"/>
+      <c r="U55" s="31"/>
+      <c r="V55" s="31"/>
+      <c r="W55" s="31"/>
+      <c r="X55" s="31"/>
+      <c r="Y55" s="31"/>
+      <c r="Z55" s="31"/>
+      <c r="AA55" s="31"/>
+      <c r="AB55" s="31"/>
+      <c r="AC55" s="31"/>
+      <c r="AD55" s="31"/>
+      <c r="AE55" s="31"/>
+      <c r="AF55" s="31"/>
+      <c r="AG55" s="31"/>
+      <c r="AH55" s="31"/>
+      <c r="AI55" s="31"/>
+      <c r="AJ55" s="31"/>
+      <c r="AK55" s="31"/>
+      <c r="AL55" s="31"/>
+      <c r="AM55" s="31"/>
+      <c r="AN55" s="31"/>
+      <c r="AO55" s="31"/>
+      <c r="AP55" s="31"/>
+      <c r="AQ55" s="31"/>
+      <c r="AR55" s="31"/>
+      <c r="AS55" s="31"/>
+      <c r="AT55" s="31"/>
+      <c r="AU55" s="31"/>
+      <c r="AV55" s="31"/>
+      <c r="AW55" s="31"/>
+      <c r="AX55" s="31"/>
+      <c r="AY55" s="31"/>
+      <c r="AZ55" s="31"/>
+      <c r="BA55" s="31"/>
+      <c r="BB55" s="31"/>
+      <c r="BC55" s="31"/>
+      <c r="BD55" s="31"/>
+      <c r="BE55" s="31"/>
+      <c r="BF55" s="31"/>
+      <c r="BG55" s="31"/>
+      <c r="BH55" s="31"/>
+      <c r="BI55" s="31"/>
+      <c r="BJ55" s="31"/>
+      <c r="BK55" s="31"/>
+      <c r="BL55" s="31"/>
+    </row>
+    <row r="56" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="46" t="s">
+        <v>13</v>
+      </c>
+      <c r="B56" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="C56" s="28"/>
+      <c r="D56" s="29"/>
+      <c r="E56" s="70"/>
+      <c r="F56" s="71"/>
+      <c r="G56" s="30"/>
+      <c r="H56" s="30" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="I56" s="33"/>
+      <c r="J56" s="33"/>
+      <c r="K56" s="33"/>
+      <c r="L56" s="33"/>
+      <c r="M56" s="33"/>
+      <c r="N56" s="33"/>
+      <c r="O56" s="33"/>
+      <c r="P56" s="33"/>
+      <c r="Q56" s="33"/>
+      <c r="R56" s="33"/>
+      <c r="S56" s="33"/>
+      <c r="T56" s="33"/>
+      <c r="U56" s="33"/>
+      <c r="V56" s="33"/>
+      <c r="W56" s="33"/>
+      <c r="X56" s="33"/>
+      <c r="Y56" s="33"/>
+      <c r="Z56" s="33"/>
+      <c r="AA56" s="33"/>
+      <c r="AB56" s="33"/>
+      <c r="AC56" s="33"/>
+      <c r="AD56" s="33"/>
+      <c r="AE56" s="33"/>
+      <c r="AF56" s="33"/>
+      <c r="AG56" s="33"/>
+      <c r="AH56" s="33"/>
+      <c r="AI56" s="33"/>
+      <c r="AJ56" s="33"/>
+      <c r="AK56" s="33"/>
+      <c r="AL56" s="33"/>
+      <c r="AM56" s="33"/>
+      <c r="AN56" s="33"/>
+      <c r="AO56" s="33"/>
+      <c r="AP56" s="33"/>
+      <c r="AQ56" s="33"/>
+      <c r="AR56" s="33"/>
+      <c r="AS56" s="33"/>
+      <c r="AT56" s="33"/>
+      <c r="AU56" s="33"/>
+      <c r="AV56" s="33"/>
+      <c r="AW56" s="33"/>
+      <c r="AX56" s="33"/>
+      <c r="AY56" s="33"/>
+      <c r="AZ56" s="33"/>
+      <c r="BA56" s="33"/>
+      <c r="BB56" s="33"/>
+      <c r="BC56" s="33"/>
+      <c r="BD56" s="33"/>
+      <c r="BE56" s="33"/>
+      <c r="BF56" s="33"/>
+      <c r="BG56" s="33"/>
+      <c r="BH56" s="33"/>
+      <c r="BI56" s="33"/>
+      <c r="BJ56" s="33"/>
+      <c r="BK56" s="33"/>
+      <c r="BL56" s="33"/>
+    </row>
+    <row r="57" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G57" s="6"/>
+    </row>
+    <row r="58" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C58" s="11"/>
+      <c r="F58" s="47"/>
+    </row>
+    <row r="59" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C59" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -4672,7 +6421,7 @@
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
   </mergeCells>
-  <conditionalFormatting sqref="D7:D33">
+  <conditionalFormatting sqref="D7:D56">
     <cfRule type="dataBar" priority="14">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -4686,12 +6435,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I5:BL33">
+  <conditionalFormatting sqref="I5:BL56">
     <cfRule type="expression" dxfId="2" priority="33">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7:BL33">
+  <conditionalFormatting sqref="I7:BL56">
     <cfRule type="expression" dxfId="1" priority="27">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
@@ -4729,7 +6478,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D7:D33</xm:sqref>
+          <xm:sqref>D7:D56</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
chore(docs): data modeling for DER, relations are missing (might add more entities)
</commit_message>
<xml_diff>
--- a/Docs/Gantt.xlsx
+++ b/Docs/Gantt.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{427189A1-905D-4126-AEFB-755F4735B153}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA396FEA-C715-41E0-817A-1632CF5E6205}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1471,23 +1471,23 @@
     <xf numFmtId="0" fontId="0" fillId="45" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="170" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="9" fillId="0" borderId="3" xfId="9">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
       <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="9" fillId="0" borderId="3" xfId="9">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="54">
@@ -2099,8 +2099,8 @@
   <dimension ref="A1:BL59"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C22" sqref="C22"/>
+      <pane ySplit="6" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2147,106 +2147,106 @@
       <c r="B3" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="95" t="s">
+      <c r="C3" s="99" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="96"/>
-      <c r="E3" s="100">
+      <c r="D3" s="100"/>
+      <c r="E3" s="98">
         <v>45857</v>
       </c>
-      <c r="F3" s="100"/>
+      <c r="F3" s="98"/>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="95" t="s">
+      <c r="C4" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="96"/>
+      <c r="D4" s="100"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="97">
+      <c r="I4" s="95">
         <f>I5</f>
         <v>45852</v>
       </c>
-      <c r="J4" s="98"/>
-      <c r="K4" s="98"/>
-      <c r="L4" s="98"/>
-      <c r="M4" s="98"/>
-      <c r="N4" s="98"/>
-      <c r="O4" s="99"/>
-      <c r="P4" s="97">
+      <c r="J4" s="96"/>
+      <c r="K4" s="96"/>
+      <c r="L4" s="96"/>
+      <c r="M4" s="96"/>
+      <c r="N4" s="96"/>
+      <c r="O4" s="97"/>
+      <c r="P4" s="95">
         <f>P5</f>
         <v>45859</v>
       </c>
-      <c r="Q4" s="98"/>
-      <c r="R4" s="98"/>
-      <c r="S4" s="98"/>
-      <c r="T4" s="98"/>
-      <c r="U4" s="98"/>
-      <c r="V4" s="99"/>
-      <c r="W4" s="97">
+      <c r="Q4" s="96"/>
+      <c r="R4" s="96"/>
+      <c r="S4" s="96"/>
+      <c r="T4" s="96"/>
+      <c r="U4" s="96"/>
+      <c r="V4" s="97"/>
+      <c r="W4" s="95">
         <f>W5</f>
         <v>45866</v>
       </c>
-      <c r="X4" s="98"/>
-      <c r="Y4" s="98"/>
-      <c r="Z4" s="98"/>
-      <c r="AA4" s="98"/>
-      <c r="AB4" s="98"/>
-      <c r="AC4" s="99"/>
-      <c r="AD4" s="97">
+      <c r="X4" s="96"/>
+      <c r="Y4" s="96"/>
+      <c r="Z4" s="96"/>
+      <c r="AA4" s="96"/>
+      <c r="AB4" s="96"/>
+      <c r="AC4" s="97"/>
+      <c r="AD4" s="95">
         <f>AD5</f>
         <v>45873</v>
       </c>
-      <c r="AE4" s="98"/>
-      <c r="AF4" s="98"/>
-      <c r="AG4" s="98"/>
-      <c r="AH4" s="98"/>
-      <c r="AI4" s="98"/>
-      <c r="AJ4" s="99"/>
-      <c r="AK4" s="97">
+      <c r="AE4" s="96"/>
+      <c r="AF4" s="96"/>
+      <c r="AG4" s="96"/>
+      <c r="AH4" s="96"/>
+      <c r="AI4" s="96"/>
+      <c r="AJ4" s="97"/>
+      <c r="AK4" s="95">
         <f>AK5</f>
         <v>45880</v>
       </c>
-      <c r="AL4" s="98"/>
-      <c r="AM4" s="98"/>
-      <c r="AN4" s="98"/>
-      <c r="AO4" s="98"/>
-      <c r="AP4" s="98"/>
-      <c r="AQ4" s="99"/>
-      <c r="AR4" s="97">
+      <c r="AL4" s="96"/>
+      <c r="AM4" s="96"/>
+      <c r="AN4" s="96"/>
+      <c r="AO4" s="96"/>
+      <c r="AP4" s="96"/>
+      <c r="AQ4" s="97"/>
+      <c r="AR4" s="95">
         <f>AR5</f>
         <v>45887</v>
       </c>
-      <c r="AS4" s="98"/>
-      <c r="AT4" s="98"/>
-      <c r="AU4" s="98"/>
-      <c r="AV4" s="98"/>
-      <c r="AW4" s="98"/>
-      <c r="AX4" s="99"/>
-      <c r="AY4" s="97">
+      <c r="AS4" s="96"/>
+      <c r="AT4" s="96"/>
+      <c r="AU4" s="96"/>
+      <c r="AV4" s="96"/>
+      <c r="AW4" s="96"/>
+      <c r="AX4" s="97"/>
+      <c r="AY4" s="95">
         <f>AY5</f>
         <v>45894</v>
       </c>
-      <c r="AZ4" s="98"/>
-      <c r="BA4" s="98"/>
-      <c r="BB4" s="98"/>
-      <c r="BC4" s="98"/>
-      <c r="BD4" s="98"/>
-      <c r="BE4" s="99"/>
-      <c r="BF4" s="97">
+      <c r="AZ4" s="96"/>
+      <c r="BA4" s="96"/>
+      <c r="BB4" s="96"/>
+      <c r="BC4" s="96"/>
+      <c r="BD4" s="96"/>
+      <c r="BE4" s="97"/>
+      <c r="BF4" s="95">
         <f>BF5</f>
         <v>45901</v>
       </c>
-      <c r="BG4" s="98"/>
-      <c r="BH4" s="98"/>
-      <c r="BI4" s="98"/>
-      <c r="BJ4" s="98"/>
-      <c r="BK4" s="98"/>
-      <c r="BL4" s="99"/>
+      <c r="BG4" s="96"/>
+      <c r="BH4" s="96"/>
+      <c r="BI4" s="96"/>
+      <c r="BJ4" s="96"/>
+      <c r="BK4" s="96"/>
+      <c r="BL4" s="97"/>
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="46" t="s">
@@ -2882,7 +2882,7 @@
         <v>44</v>
       </c>
       <c r="D9" s="17">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="E9" s="77">
         <f>Inicio_del_proyecto</f>
@@ -2962,10 +2962,10 @@
         <v>53</v>
       </c>
       <c r="C10" s="53" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="D10" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" s="77">
         <f>Inicio_del_proyecto</f>
@@ -6409,17 +6409,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
+    <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="I4:O4"/>
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
-    <mergeCell ref="AY4:BE4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D56">
     <cfRule type="dataBar" priority="14">
@@ -6590,6 +6590,35 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="24" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2d714a3296df14eba7a100bb665443ca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="49549bf45bfbbfb6cffed527380e77e1" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -6877,36 +6906,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC3AD2E1-977A-4D4F-8EE8-D64B5FFADF75}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4A34E49-7289-4AEA-9593-4F55E04ADB10}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F80F839-78EF-4FF4-A673-3CC84279C232}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6925,24 +6945,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4A34E49-7289-4AEA-9593-4F55E04ADB10}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC3AD2E1-977A-4D4F-8EE8-D64B5FFADF75}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>